<commit_message>
update templaate, remove data and update sheet names and starting cells
</commit_message>
<xml_diff>
--- a/signin_templates/manager_signin.xlsx
+++ b/signin_templates/manager_signin.xlsx
@@ -8,24 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brendanwoo/projects/sro_sign_in/signin_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60310A4C-2AA8-4249-895C-923E97F485BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7937D726-B971-514B-8D52-486AB1F4029A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{542D648B-9180-43EF-9053-182057C63D4C}"/>
+    <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="5" xr2:uid="{542D648B-9180-43EF-9053-182057C63D4C}"/>
   </bookViews>
   <sheets>
     <sheet name="GTWCA" sheetId="1" r:id="rId1"/>
-    <sheet name="GTAM" sheetId="5" r:id="rId2"/>
-    <sheet name="GT4A" sheetId="6" r:id="rId3"/>
-    <sheet name="TC" sheetId="7" r:id="rId4"/>
+    <sheet name="PGT4A" sheetId="6" r:id="rId2"/>
+    <sheet name="GTAM" sheetId="5" r:id="rId3"/>
+    <sheet name="TCAM" sheetId="7" r:id="rId4"/>
     <sheet name="GR Cup" sheetId="8" r:id="rId5"/>
-    <sheet name="Event Log" sheetId="9" r:id="rId6"/>
+    <sheet name="Event_log" sheetId="9" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="4">'GR Cup'!$A$1:$D$22</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">GT4A!$A$1:$D$28</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">GTAM!$A$1:$D$28</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">GTAM!$A$1:$D$28</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">GTWCA!$A$2:$D$24</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">TC!$A$4:$D$22</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">PGT4A!$A$1:$D$29</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">TCAM!$A$4:$D$23</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="42">
   <si>
     <t>Car #</t>
   </si>
@@ -54,172 +54,19 @@
     <t xml:space="preserve">Team </t>
   </si>
   <si>
-    <t>04</t>
-  </si>
-  <si>
-    <t>Crowdstrike by Riley</t>
-  </si>
-  <si>
-    <t>DXDT Racing</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>Conquest Racing</t>
-  </si>
-  <si>
-    <t>RS1</t>
-  </si>
-  <si>
-    <t>Triarsi Competizione</t>
-  </si>
-  <si>
-    <t>ST Racing</t>
-  </si>
-  <si>
-    <t>RealTime Racing</t>
-  </si>
-  <si>
-    <t>Wright Motorsports</t>
-  </si>
-  <si>
-    <t>MDK Motorsports</t>
-  </si>
-  <si>
-    <t>Racers Edge Motorsports</t>
-  </si>
-  <si>
-    <t>BimmerWorld</t>
-  </si>
-  <si>
-    <t>CRP Racing</t>
-  </si>
-  <si>
-    <t>043</t>
-  </si>
-  <si>
-    <t>OnlyFans Racing with P1 Groupe by MRS</t>
-  </si>
-  <si>
-    <t>TKO Motorsports</t>
-  </si>
-  <si>
-    <t>Flying Lizard Motorsports</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>Blackdog Speed Shop</t>
-  </si>
-  <si>
-    <t>Carrus Callas Raceteam</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>Heart of Racing Team</t>
-  </si>
-  <si>
-    <t>50</t>
-  </si>
-  <si>
-    <t>Chouest Povoledo Racing</t>
-  </si>
-  <si>
     <t>69</t>
-  </si>
-  <si>
-    <t>Rotek Racing</t>
-  </si>
-  <si>
-    <t>Auto Technic Racing</t>
-  </si>
-  <si>
-    <t>ACI Motorsports</t>
-  </si>
-  <si>
-    <t>09</t>
-  </si>
-  <si>
-    <t>Zotz Racing/ CCDP Racing</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>Techsport Racing</t>
   </si>
   <si>
     <t>23</t>
   </si>
   <si>
-    <t>Conquest Racing / JMF Motorsport</t>
-  </si>
-  <si>
-    <t>37</t>
-  </si>
-  <si>
     <t>Skip Barber Racing School</t>
-  </si>
-  <si>
-    <t>44</t>
-  </si>
-  <si>
-    <t>Rooster Hall Racing</t>
-  </si>
-  <si>
-    <t>NOLASPORT</t>
   </si>
   <si>
     <t>Smooge Racing</t>
   </si>
   <si>
-    <t>STR38 Motorsports</t>
-  </si>
-  <si>
-    <t>89</t>
-  </si>
-  <si>
-    <t>RENNtech Motorsports</t>
-  </si>
-  <si>
-    <t>Random Vandals Racing</t>
-  </si>
-  <si>
-    <t>999</t>
-  </si>
-  <si>
-    <t>Hanley Motorsports</t>
-  </si>
-  <si>
-    <t>AOA Racing</t>
-  </si>
-  <si>
-    <t>Fast Track Racing</t>
-  </si>
-  <si>
-    <t>Rigid Speed Company</t>
-  </si>
-  <si>
-    <t>LA Honda World Racing</t>
-  </si>
-  <si>
     <t>VGRT</t>
-  </si>
-  <si>
-    <t>MINI JCW Team</t>
-  </si>
-  <si>
-    <t>Genracer / Ricca Autosport</t>
-  </si>
-  <si>
-    <t>TechSport Racing</t>
   </si>
   <si>
     <t>March 30-April 2</t>
@@ -285,15 +132,6 @@
     <t>TC Team Manager Sign In</t>
   </si>
   <si>
-    <t>22, 23</t>
-  </si>
-  <si>
-    <t>24, 26</t>
-  </si>
-  <si>
-    <t>78, 780</t>
-  </si>
-  <si>
     <t>27, 28</t>
   </si>
   <si>
@@ -309,76 +147,10 @@
     <t>11, 31</t>
   </si>
   <si>
-    <t>27, 41</t>
-  </si>
-  <si>
-    <t>88, 438</t>
-  </si>
-  <si>
-    <t>92,  98</t>
-  </si>
-  <si>
-    <t>51, 253</t>
-  </si>
-  <si>
-    <t>67, 68</t>
-  </si>
-  <si>
-    <t>36, 82</t>
-  </si>
-  <si>
-    <t>7 , 19, 58</t>
-  </si>
-  <si>
-    <t>47, 52, 83</t>
-  </si>
-  <si>
-    <t>72</t>
-  </si>
-  <si>
-    <t>KRUGSPEED</t>
-  </si>
-  <si>
-    <t>SKI Autosport</t>
-  </si>
-  <si>
-    <t>7, 19, 34, 77</t>
-  </si>
-  <si>
-    <t>TRG - The Racers Group</t>
-  </si>
-  <si>
     <t>Event Logistics Briefing</t>
   </si>
   <si>
-    <t>Ian Lacy Racing</t>
-  </si>
-  <si>
-    <t>099</t>
-  </si>
-  <si>
-    <t>MISHUMOTORS</t>
-  </si>
-  <si>
     <t>Pura Vida Team</t>
-  </si>
-  <si>
-    <t>TRG -The Racers Group</t>
-  </si>
-  <si>
-    <t>009</t>
-  </si>
-  <si>
-    <t>Archangel Motorsports</t>
-  </si>
-  <si>
-    <t>045</t>
-  </si>
-  <si>
-    <t>34, 35</t>
-  </si>
-  <si>
-    <t xml:space="preserve">44 </t>
   </si>
   <si>
     <t>5, 55</t>
@@ -387,61 +159,7 @@
     <t>7, 30</t>
   </si>
   <si>
-    <t>08</t>
-  </si>
-  <si>
-    <t>BGB Motorsports</t>
-  </si>
-  <si>
-    <t>81</t>
-  </si>
-  <si>
-    <t>09, 21</t>
-  </si>
-  <si>
-    <t>5, 07</t>
-  </si>
-  <si>
-    <t>8, 99</t>
-  </si>
-  <si>
     <t>2, 37, 73</t>
-  </si>
-  <si>
-    <t>Lone Star Racing / Mad Joker</t>
-  </si>
-  <si>
-    <t>GMG Racing</t>
-  </si>
-  <si>
-    <t>Lone Star Racing</t>
-  </si>
-  <si>
-    <t>32, 58</t>
-  </si>
-  <si>
-    <t>Chicago Performance &amp; Tuning, Co.</t>
-  </si>
-  <si>
-    <t>2, 8, 13</t>
-  </si>
-  <si>
-    <t>van der Steur Racing</t>
-  </si>
-  <si>
-    <t>428</t>
-  </si>
-  <si>
-    <t>14, 808</t>
-  </si>
-  <si>
-    <t>DRS</t>
-  </si>
-  <si>
-    <t>Ascent Racing</t>
-  </si>
-  <si>
-    <t>37, 60, 62, 63</t>
   </si>
   <si>
     <t>18, 76</t>
@@ -451,9 +169,6 @@
   </si>
   <si>
     <t>88, 98</t>
-  </si>
-  <si>
-    <t>011, 80</t>
   </si>
   <si>
     <t>Print Name</t>
@@ -780,7 +495,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -839,17 +554,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -1068,6 +772,56 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1075,7 +829,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="189">
+  <cellXfs count="198">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1119,16 +873,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1144,22 +898,22 @@
     <xf numFmtId="49" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1188,7 +942,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1197,10 +951,10 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1209,19 +963,19 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="26" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1236,46 +990,46 @@
     <xf numFmtId="49" fontId="28" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="30" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1287,13 +1041,13 @@
     <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1302,7 +1056,7 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="21" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1323,88 +1077,76 @@
     <xf numFmtId="49" fontId="32" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="33" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="32" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="31" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="31" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="35" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="35" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="36" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="31" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="31" fillId="0" borderId="20" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="31" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="35" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="32" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="33" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="34" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="33" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="32" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="32" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="31" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="31" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="35" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="35" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="36" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="31" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="31" fillId="0" borderId="21" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="31" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="35" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="32" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="33" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="34" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="33" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="32" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="32" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="33" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1416,70 +1158,61 @@
     <xf numFmtId="49" fontId="34" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="32" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="32" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="32" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="32" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="33" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="32" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="33" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="37" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="37" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="38" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="38" fillId="0" borderId="17" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="37" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="38" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="38" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="37" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="37" fillId="0" borderId="20" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="34" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="37" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="34" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1488,19 +1221,19 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="40" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1518,15 +1251,15 @@
     <xf numFmtId="49" fontId="41" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="40" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="40" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="40" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1539,22 +1272,22 @@
     <xf numFmtId="49" fontId="41" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="41" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="42" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="41" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="42" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="41" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="41" fillId="0" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="42" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="41" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="42" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="41" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="43" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1563,12 +1296,12 @@
     <xf numFmtId="0" fontId="39" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1583,30 +1316,22 @@
     <xf numFmtId="49" fontId="39" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="37" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="1" fontId="37" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="31" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="35" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="31" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1614,15 +1339,61 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="31" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="35" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="31" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="33" fillId="0" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="32" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="32" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="32" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="25" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="34" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="34" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -2874,6 +2645,61 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
+      <xdr:rowOff>19538</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2938510</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>144831</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4294C48-A863-3549-A59D-CC438285C40C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="644770" y="214923"/>
+          <a:ext cx="2937289" cy="691908"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>223631</xdr:rowOff>
     </xdr:from>
     <xdr:to>
@@ -2922,75 +2748,20 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>19538</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>2938510</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>144831</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4294C48-A863-3549-A59D-CC438285C40C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="644770" y="214923"/>
-          <a:ext cx="2937289" cy="691908"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>302148</xdr:rowOff>
+      <xdr:colOff>36286</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>157006</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>91034</xdr:colOff>
+      <xdr:colOff>127320</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>524926</xdr:rowOff>
+      <xdr:rowOff>180212</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3019,8 +2790,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="76506" y="669377"/>
-          <a:ext cx="2937058" cy="528802"/>
+          <a:off x="36286" y="356577"/>
+          <a:ext cx="2939463" cy="531206"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3097,6 +2868,21 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{56F25BC1-6701-4669-AC0F-E1673995674A}" name="Table2267" displayName="Table2267" ref="A7:D29" totalsRowShown="0" headerRowDxfId="28" headerRowBorderDxfId="27" tableBorderDxfId="26" totalsRowBorderDxfId="25">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:D29">
+    <sortCondition ref="A7:A29"/>
+  </sortState>
+  <tableColumns count="4">
+    <tableColumn id="3" xr3:uid="{C0375D1B-A6A9-4878-94F1-144B367DBFAE}" name="Team " dataDxfId="24" dataCellStyle="Neutral"/>
+    <tableColumn id="1" xr3:uid="{72AB2F61-1891-C246-9F82-F99E634034BF}" name="Car #" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{731AF936-9BBC-4114-AF94-6737C2C799AD}" name="Print Name" dataDxfId="22" dataCellStyle="Neutral"/>
+    <tableColumn id="5" xr3:uid="{4AAAC599-A742-4343-8BE4-F0207EAEB236}" name="Signature" dataDxfId="21" dataCellStyle="Neutral"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{EEF14E4E-087A-46C7-831D-A668229E00D6}" name="Table226" displayName="Table226" ref="A7:D28" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:D28">
     <sortCondition ref="A7:A28"/>
@@ -3111,25 +2897,10 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{56F25BC1-6701-4669-AC0F-E1673995674A}" name="Table2267" displayName="Table2267" ref="A6:D28" totalsRowShown="0" headerRowDxfId="28" headerRowBorderDxfId="27" tableBorderDxfId="26" totalsRowBorderDxfId="25">
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:D28">
-    <sortCondition ref="A6:A28"/>
-  </sortState>
-  <tableColumns count="4">
-    <tableColumn id="3" xr3:uid="{C0375D1B-A6A9-4878-94F1-144B367DBFAE}" name="Team " dataDxfId="24" dataCellStyle="Neutral"/>
-    <tableColumn id="1" xr3:uid="{72AB2F61-1891-C246-9F82-F99E634034BF}" name="Car #" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{731AF936-9BBC-4114-AF94-6737C2C799AD}" name="Team Manager - Print Name" dataDxfId="22" dataCellStyle="Neutral"/>
-    <tableColumn id="5" xr3:uid="{4AAAC599-A742-4343-8BE4-F0207EAEB236}" name="Signature" dataDxfId="21" dataCellStyle="Neutral"/>
-  </tableColumns>
-  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{7C975FDB-E1BE-412D-9026-C8BCE6F82D94}" name="Table2268" displayName="Table2268" ref="A6:D19" totalsRowShown="0" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19" tableBorderDxfId="17" totalsRowBorderDxfId="16">
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:D19">
-    <sortCondition ref="A7:A19"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{7C975FDB-E1BE-412D-9026-C8BCE6F82D94}" name="Table2268" displayName="Table2268" ref="A7:D20" totalsRowShown="0" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:D20">
+    <sortCondition ref="A8:A20"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="3" xr3:uid="{9A87D9F1-DEF9-4884-AF55-85CDAB8CC5A8}" name="Team " dataDxfId="15" dataCellStyle="Neutral"/>
@@ -3165,7 +2936,7 @@
   </sortState>
   <tableColumns count="3">
     <tableColumn id="2" xr3:uid="{AD000ADB-6327-CD45-BE99-F1047C0BF216}" name="Team " dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{CDB7A7EE-F7C4-DE41-B5A3-3A45AA9CEAAC}" name="Team Manager - Print Name"/>
+    <tableColumn id="3" xr3:uid="{CDB7A7EE-F7C4-DE41-B5A3-3A45AA9CEAAC}" name="Print Name"/>
     <tableColumn id="4" xr3:uid="{66076889-B43A-3746-B4F7-4CFF3E5423AA}" name="Signature" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3488,18 +3259,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="177"/>
+      <c r="A2" s="173"/>
       <c r="B2" s="68"/>
-      <c r="C2" s="185" t="s">
-        <v>76</v>
-      </c>
-      <c r="D2" s="185"/>
+      <c r="C2" s="169" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="169"/>
     </row>
     <row r="3" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="177"/>
+      <c r="A3" s="173"/>
       <c r="B3" s="68"/>
-      <c r="C3" s="185"/>
-      <c r="D3" s="185"/>
+      <c r="C3" s="169"/>
+      <c r="D3" s="169"/>
     </row>
     <row r="7" spans="1:4" s="19" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="53" t="s">
@@ -3509,105 +3280,105 @@
         <v>0</v>
       </c>
       <c r="C7" s="53" t="s">
-        <v>136</v>
+        <v>41</v>
       </c>
       <c r="D7" s="53" t="s">
-        <v>74</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="19" customFormat="1" ht="43" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="91"/>
-      <c r="B8" s="92"/>
+      <c r="A8" s="87"/>
+      <c r="B8" s="88"/>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
     </row>
     <row r="9" spans="1:4" s="19" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="93"/>
-      <c r="B9" s="94"/>
+      <c r="A9" s="89"/>
+      <c r="B9" s="90"/>
       <c r="C9" s="21"/>
       <c r="D9" s="21"/>
     </row>
     <row r="10" spans="1:4" s="19" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="93"/>
-      <c r="B10" s="94"/>
+      <c r="A10" s="89"/>
+      <c r="B10" s="90"/>
       <c r="C10" s="22"/>
       <c r="D10" s="22"/>
     </row>
     <row r="11" spans="1:4" s="19" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="95"/>
-      <c r="B11" s="92"/>
+      <c r="A11" s="91"/>
+      <c r="B11" s="88"/>
       <c r="C11" s="21"/>
       <c r="D11" s="21"/>
     </row>
     <row r="12" spans="1:4" s="19" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="93"/>
-      <c r="B12" s="94"/>
+      <c r="A12" s="89"/>
+      <c r="B12" s="90"/>
       <c r="C12" s="20"/>
       <c r="D12" s="21"/>
     </row>
     <row r="13" spans="1:4" s="19" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="96"/>
-      <c r="B13" s="92"/>
+      <c r="A13" s="92"/>
+      <c r="B13" s="88"/>
       <c r="C13" s="21"/>
       <c r="D13" s="21"/>
     </row>
     <row r="14" spans="1:4" s="19" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="93"/>
-      <c r="B14" s="92"/>
+      <c r="A14" s="89"/>
+      <c r="B14" s="88"/>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
     </row>
     <row r="15" spans="1:4" s="19" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="95"/>
-      <c r="B15" s="94"/>
+      <c r="A15" s="91"/>
+      <c r="B15" s="90"/>
       <c r="C15" s="21"/>
       <c r="D15" s="21"/>
     </row>
     <row r="16" spans="1:4" s="19" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="93"/>
-      <c r="B16" s="94"/>
+      <c r="A16" s="89"/>
+      <c r="B16" s="90"/>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
     </row>
     <row r="17" spans="1:4" s="19" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="97"/>
-      <c r="B17" s="98"/>
+      <c r="A17" s="93"/>
+      <c r="B17" s="94"/>
       <c r="C17" s="75"/>
       <c r="D17" s="23"/>
     </row>
     <row r="18" spans="1:4" s="19" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="99"/>
-      <c r="B18" s="94"/>
+      <c r="A18" s="95"/>
+      <c r="B18" s="90"/>
       <c r="C18" s="74"/>
       <c r="D18" s="22"/>
     </row>
     <row r="19" spans="1:4" s="19" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="100"/>
-      <c r="B19" s="94"/>
+      <c r="A19" s="96"/>
+      <c r="B19" s="90"/>
       <c r="C19" s="20"/>
       <c r="D19" s="20"/>
     </row>
     <row r="20" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A20" s="93"/>
-      <c r="B20" s="186"/>
+      <c r="A20" s="89"/>
+      <c r="B20" s="170"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
     </row>
     <row r="21" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A21" s="93"/>
-      <c r="B21" s="186"/>
+      <c r="A21" s="89"/>
+      <c r="B21" s="170"/>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
     </row>
     <row r="22" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A22" s="93"/>
-      <c r="B22" s="186"/>
+      <c r="A22" s="89"/>
+      <c r="B22" s="170"/>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
     </row>
     <row r="23" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A23" s="187"/>
-      <c r="B23" s="188"/>
+      <c r="A23" s="171"/>
+      <c r="B23" s="172"/>
       <c r="C23" s="11"/>
       <c r="D23" s="11"/>
     </row>
@@ -3625,14 +3396,205 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26B660E4-5CC7-4B8C-B888-8D9BEEB0F61E}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:D29"/>
+  <sheetViews>
+    <sheetView view="pageLayout" zoomScale="60" zoomScaleNormal="115" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="4.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="52.83203125" customWidth="1"/>
+    <col min="2" max="2" width="29" customWidth="1"/>
+    <col min="3" max="3" width="54" customWidth="1"/>
+    <col min="4" max="4" width="50.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="68"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="178" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="178"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C3" s="179"/>
+      <c r="D3" s="179"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C4" s="179"/>
+      <c r="D4" s="179"/>
+    </row>
+    <row r="7" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="50.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="103"/>
+      <c r="B8" s="104"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="12"/>
+    </row>
+    <row r="9" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="105"/>
+      <c r="B9" s="106"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="38"/>
+    </row>
+    <row r="10" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="112"/>
+      <c r="B10" s="131"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="86"/>
+      <c r="B11" s="107"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+    </row>
+    <row r="12" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="86"/>
+      <c r="B12" s="108"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="12"/>
+    </row>
+    <row r="13" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="109"/>
+      <c r="B13" s="110"/>
+      <c r="C13" s="97"/>
+      <c r="D13" s="99"/>
+    </row>
+    <row r="14" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="102"/>
+      <c r="B14" s="111"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="7"/>
+    </row>
+    <row r="15" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="180"/>
+      <c r="B15" s="111"/>
+      <c r="C15" s="188"/>
+      <c r="D15" s="9"/>
+    </row>
+    <row r="16" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="181"/>
+      <c r="B16" s="108"/>
+      <c r="C16" s="189"/>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="182"/>
+      <c r="B17" s="111"/>
+      <c r="C17" s="188"/>
+      <c r="D17" s="98"/>
+    </row>
+    <row r="18" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="180"/>
+      <c r="B18" s="113"/>
+      <c r="C18" s="188"/>
+      <c r="D18" s="12"/>
+    </row>
+    <row r="19" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="183"/>
+      <c r="B19" s="108"/>
+      <c r="C19" s="189"/>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="180"/>
+      <c r="B20" s="114"/>
+      <c r="C20" s="188"/>
+      <c r="D20" s="9"/>
+    </row>
+    <row r="21" spans="1:4" s="36" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="182"/>
+      <c r="B21" s="108"/>
+      <c r="C21" s="188"/>
+      <c r="D21" s="9"/>
+    </row>
+    <row r="22" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="180"/>
+      <c r="B22" s="111"/>
+      <c r="C22" s="190"/>
+      <c r="D22" s="12"/>
+    </row>
+    <row r="23" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="184"/>
+      <c r="B23" s="111"/>
+      <c r="C23" s="188"/>
+      <c r="D23" s="12"/>
+    </row>
+    <row r="24" spans="1:4" s="1" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="185"/>
+      <c r="B24" s="108"/>
+      <c r="C24" s="191"/>
+      <c r="D24" s="77"/>
+    </row>
+    <row r="25" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="186"/>
+      <c r="B25" s="108"/>
+      <c r="C25" s="192"/>
+      <c r="D25" s="12"/>
+    </row>
+    <row r="26" spans="1:4" s="36" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="181"/>
+      <c r="B26" s="194"/>
+      <c r="C26" s="193"/>
+      <c r="D26" s="38"/>
+    </row>
+    <row r="27" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="181"/>
+      <c r="B27" s="194"/>
+      <c r="C27" s="193"/>
+      <c r="D27" s="38"/>
+    </row>
+    <row r="28" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="187"/>
+      <c r="B28" s="195"/>
+      <c r="C28" s="189"/>
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="115"/>
+      <c r="B29" s="116"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="27"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="61" fitToHeight="2" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85FEBD50-9ECF-4D52-B6BF-7430521747DA}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A2" zoomScale="60" zoomScaleNormal="115" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView view="pageLayout" zoomScale="60" zoomScaleNormal="115" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3644,26 +3606,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="177"/>
+      <c r="A2" s="173"/>
       <c r="B2" s="68"/>
     </row>
     <row r="3" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="177"/>
+      <c r="A3" s="173"/>
       <c r="B3" s="68"/>
-      <c r="C3" s="178" t="s">
-        <v>77</v>
-      </c>
-      <c r="D3" s="178"/>
+      <c r="C3" s="176" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="176"/>
     </row>
     <row r="4" spans="1:4" ht="26" x14ac:dyDescent="0.3">
-      <c r="C4" s="178"/>
-      <c r="D4" s="178"/>
+      <c r="C4" s="176"/>
+      <c r="D4" s="176"/>
     </row>
     <row r="5" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="179"/>
-      <c r="B5" s="179"/>
-      <c r="C5" s="179"/>
-      <c r="D5" s="179"/>
+      <c r="A5" s="177"/>
+      <c r="B5" s="177"/>
+      <c r="C5" s="177"/>
+      <c r="D5" s="177"/>
     </row>
     <row r="7" spans="1:4" s="1" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
@@ -3673,219 +3635,135 @@
         <v>0</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>75</v>
+        <v>24</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>74</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="5" customFormat="1" ht="36" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="55" t="s">
-        <v>107</v>
-      </c>
-      <c r="B8" s="81" t="s">
-        <v>108</v>
-      </c>
+      <c r="A8" s="55"/>
+      <c r="B8" s="81"/>
       <c r="C8" s="9"/>
       <c r="D8" s="13"/>
     </row>
     <row r="9" spans="1:4" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="73" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="81" t="s">
-        <v>20</v>
-      </c>
+      <c r="A9" s="73"/>
+      <c r="B9" s="81"/>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
     </row>
     <row r="10" spans="1:4" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="55" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="81" t="s">
-        <v>5</v>
-      </c>
+      <c r="A10" s="55"/>
+      <c r="B10" s="81"/>
       <c r="C10" s="9"/>
       <c r="D10" s="7"/>
     </row>
     <row r="11" spans="1:4" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="174" t="s">
-        <v>124</v>
-      </c>
-      <c r="B11" s="81">
-        <v>94</v>
-      </c>
+      <c r="A11" s="167"/>
+      <c r="B11" s="81"/>
       <c r="C11" s="9"/>
       <c r="D11" s="13"/>
     </row>
     <row r="12" spans="1:4" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="73" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="81" t="s">
-        <v>25</v>
-      </c>
+      <c r="A12" s="73"/>
+      <c r="B12" s="81"/>
       <c r="C12" s="8"/>
       <c r="D12" s="7"/>
     </row>
     <row r="13" spans="1:4" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="55" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="54" t="s">
-        <v>2</v>
-      </c>
+      <c r="A13" s="55"/>
+      <c r="B13" s="54"/>
       <c r="C13" s="9"/>
       <c r="D13" s="76"/>
     </row>
     <row r="14" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="72" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="82" t="s">
-        <v>87</v>
-      </c>
+      <c r="A14" s="72"/>
+      <c r="B14" s="82"/>
       <c r="C14" s="9"/>
       <c r="D14" s="80"/>
     </row>
     <row r="15" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="55" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="81" t="s">
-        <v>113</v>
-      </c>
+      <c r="A15" s="55"/>
+      <c r="B15" s="81"/>
       <c r="C15" s="9"/>
       <c r="D15" s="76"/>
     </row>
     <row r="16" spans="1:4" s="36" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="55" t="s">
-        <v>51</v>
-      </c>
-      <c r="B16" s="81">
-        <v>11</v>
-      </c>
+      <c r="A16" s="55"/>
+      <c r="B16" s="81"/>
       <c r="C16" s="9"/>
       <c r="D16" s="76"/>
     </row>
     <row r="17" spans="1:4" s="36" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="83" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="84" t="s">
-        <v>125</v>
-      </c>
+      <c r="A17" s="83"/>
+      <c r="B17" s="84"/>
       <c r="C17" s="34"/>
       <c r="D17" s="13"/>
     </row>
     <row r="18" spans="1:4" s="36" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="83" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="84">
-        <v>460</v>
-      </c>
+      <c r="A18" s="83"/>
+      <c r="B18" s="84"/>
       <c r="C18" s="9"/>
       <c r="D18" s="13"/>
     </row>
     <row r="19" spans="1:4" s="36" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="55" t="s">
-        <v>121</v>
-      </c>
-      <c r="B19" s="172" t="s">
-        <v>123</v>
-      </c>
+      <c r="A19" s="55"/>
+      <c r="B19" s="165"/>
       <c r="C19" s="9"/>
       <c r="D19" s="13"/>
     </row>
     <row r="20" spans="1:4" s="36" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="72" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" s="82" t="s">
-        <v>23</v>
-      </c>
+      <c r="A20" s="72"/>
+      <c r="B20" s="82"/>
       <c r="C20" s="9"/>
       <c r="D20" s="76"/>
     </row>
     <row r="21" spans="1:4" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="55" t="s">
-        <v>120</v>
-      </c>
-      <c r="B21" s="81" t="s">
-        <v>135</v>
-      </c>
+      <c r="A21" s="55"/>
+      <c r="B21" s="81"/>
       <c r="C21" s="9"/>
       <c r="D21" s="76"/>
     </row>
     <row r="22" spans="1:4" s="35" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="85" t="s">
-        <v>103</v>
-      </c>
-      <c r="B22" s="81">
-        <v>70</v>
-      </c>
+      <c r="A22" s="85"/>
+      <c r="B22" s="81"/>
       <c r="C22" s="9"/>
       <c r="D22" s="78"/>
     </row>
     <row r="23" spans="1:4" s="35" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="52" t="s">
-        <v>17</v>
-      </c>
-      <c r="B23" s="82" t="s">
-        <v>16</v>
-      </c>
+      <c r="A23" s="52"/>
+      <c r="B23" s="82"/>
       <c r="C23" s="9"/>
       <c r="D23" s="13"/>
     </row>
     <row r="24" spans="1:4" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="85" t="s">
-        <v>28</v>
-      </c>
-      <c r="B24" s="81" t="s">
-        <v>102</v>
-      </c>
+      <c r="A24" s="85"/>
+      <c r="B24" s="81"/>
       <c r="C24" s="9"/>
       <c r="D24" s="77"/>
     </row>
     <row r="25" spans="1:4" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="55" t="s">
-        <v>97</v>
-      </c>
-      <c r="B25" s="84">
-        <v>3</v>
-      </c>
+      <c r="A25" s="55"/>
+      <c r="B25" s="84"/>
       <c r="C25" s="9"/>
       <c r="D25" s="13"/>
     </row>
     <row r="26" spans="1:4" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="83" t="s">
-        <v>18</v>
-      </c>
-      <c r="B26" s="84">
-        <v>101</v>
-      </c>
+      <c r="A26" s="83"/>
+      <c r="B26" s="84"/>
       <c r="C26" s="34"/>
       <c r="D26" s="47"/>
     </row>
     <row r="27" spans="1:4" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="55" t="s">
-        <v>105</v>
-      </c>
-      <c r="B27" s="81" t="s">
-        <v>106</v>
-      </c>
+      <c r="A27" s="55"/>
+      <c r="B27" s="81"/>
       <c r="C27" s="9"/>
       <c r="D27" s="13"/>
     </row>
     <row r="28" spans="1:4" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="55" t="s">
-        <v>11</v>
-      </c>
-      <c r="B28" s="81">
-        <v>120</v>
-      </c>
+      <c r="A28" s="55"/>
+      <c r="B28" s="81"/>
       <c r="C28" s="9"/>
       <c r="D28" s="79"/>
     </row>
@@ -3902,11 +3780,8 @@
       <c r="D30" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="1">
     <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
   </mergeCells>
   <phoneticPr fontId="45" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.45185185185185184" header="0.3" footer="0.3"/>
@@ -3922,294 +3797,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26B660E4-5CC7-4B8C-B888-8D9BEEB0F61E}">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A2:D28"/>
-  <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A14" zoomScale="60" zoomScaleNormal="115" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="4.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="52.83203125" customWidth="1"/>
-    <col min="2" max="2" width="29" customWidth="1"/>
-    <col min="3" max="3" width="54" customWidth="1"/>
-    <col min="4" max="4" width="50.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="68"/>
-      <c r="B2" s="68"/>
-      <c r="C2" s="180" t="s">
-        <v>77</v>
-      </c>
-      <c r="D2" s="180"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C3" s="177"/>
-      <c r="D3" s="177"/>
-    </row>
-    <row r="6" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="50.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="107" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="108" t="s">
-        <v>93</v>
-      </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="12"/>
-    </row>
-    <row r="8" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="109" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="110" t="s">
-        <v>90</v>
-      </c>
-      <c r="C8" s="37"/>
-      <c r="D8" s="38"/>
-    </row>
-    <row r="9" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="116" t="s">
-        <v>114</v>
-      </c>
-      <c r="B9" s="138" t="s">
-        <v>115</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="86" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="111" t="s">
-        <v>92</v>
-      </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-    </row>
-    <row r="11" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="86" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="112" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="12"/>
-    </row>
-    <row r="12" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="113" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="114" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="101"/>
-      <c r="D12" s="103"/>
-    </row>
-    <row r="13" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="106" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="115" t="s">
-        <v>109</v>
-      </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="7"/>
-    </row>
-    <row r="14" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="87" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="115" t="s">
-        <v>125</v>
-      </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-    </row>
-    <row r="15" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="109" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15" s="112" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="86" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="115" t="s">
-        <v>80</v>
-      </c>
-      <c r="C16" s="9"/>
-      <c r="D16" s="102"/>
-    </row>
-    <row r="17" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="87" t="s">
-        <v>96</v>
-      </c>
-      <c r="B17" s="117" t="s">
-        <v>95</v>
-      </c>
-      <c r="C17" s="9"/>
-      <c r="D17" s="12"/>
-    </row>
-    <row r="18" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="118" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" s="112" t="s">
-        <v>94</v>
-      </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="87" t="s">
-        <v>47</v>
-      </c>
-      <c r="B19" s="119" t="s">
-        <v>89</v>
-      </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-    </row>
-    <row r="20" spans="1:4" s="36" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="86" t="s">
-        <v>46</v>
-      </c>
-      <c r="B20" s="120" t="s">
-        <v>45</v>
-      </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-    </row>
-    <row r="21" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="87" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21" s="108" t="s">
-        <v>110</v>
-      </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="12"/>
-    </row>
-    <row r="22" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="88" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22" s="108" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="12"/>
-    </row>
-    <row r="23" spans="1:4" s="1" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="89" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" s="121" t="s">
-        <v>38</v>
-      </c>
-      <c r="C23" s="77"/>
-      <c r="D23" s="77"/>
-    </row>
-    <row r="24" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="90" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" s="122" t="s">
-        <v>91</v>
-      </c>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-    </row>
-    <row r="25" spans="1:4" s="36" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="109" t="s">
-        <v>44</v>
-      </c>
-      <c r="B25" s="110" t="s">
-        <v>88</v>
-      </c>
-      <c r="C25" s="37"/>
-      <c r="D25" s="38"/>
-    </row>
-    <row r="26" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="109" t="s">
-        <v>35</v>
-      </c>
-      <c r="B26" s="110" t="s">
-        <v>79</v>
-      </c>
-      <c r="C26" s="37"/>
-      <c r="D26" s="38"/>
-    </row>
-    <row r="27" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="116" t="s">
-        <v>126</v>
-      </c>
-      <c r="B27" s="175" t="s">
-        <v>127</v>
-      </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="4"/>
-    </row>
-    <row r="28" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="121" t="s">
-        <v>32</v>
-      </c>
-      <c r="B28" s="123" t="s">
-        <v>31</v>
-      </c>
-      <c r="C28" s="26"/>
-      <c r="D28" s="27"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="61" fitToHeight="2" orientation="landscape" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <tableParts count="1">
-    <tablePart r:id="rId3"/>
-  </tableParts>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A65A0B2D-D47A-4F44-8AFC-080610D14133}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A3:CJ19"/>
+  <dimension ref="A3:CJ20"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A2" zoomScale="60" zoomScaleNormal="115" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView view="pageLayout" zoomScale="70" zoomScaleNormal="115" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4222,129 +3818,39 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:88" ht="24" x14ac:dyDescent="0.3">
-      <c r="C3" s="181" t="s">
-        <v>78</v>
-      </c>
-      <c r="D3" s="181"/>
+      <c r="C3" s="197" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="197"/>
     </row>
     <row r="4" spans="1:88" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="182"/>
-      <c r="D4" s="182"/>
-    </row>
-    <row r="5" spans="1:88" x14ac:dyDescent="0.2">
-      <c r="F5" s="177"/>
-      <c r="G5" s="177"/>
-    </row>
-    <row r="6" spans="1:88" s="18" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="49" t="s">
+      <c r="C4" s="196"/>
+      <c r="D4" s="196"/>
+    </row>
+    <row r="5" spans="1:88" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C5" s="196"/>
+      <c r="D5" s="196"/>
+    </row>
+    <row r="6" spans="1:88" x14ac:dyDescent="0.2">
+      <c r="F6" s="173"/>
+      <c r="G6" s="173"/>
+    </row>
+    <row r="7" spans="1:88" s="18" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="49" t="s">
+      <c r="B7" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="50" t="s">
-        <v>75</v>
-      </c>
-      <c r="D6" s="49" t="s">
-        <v>74</v>
-      </c>
-      <c r="E6" s="39"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="39"/>
-      <c r="K6" s="39"/>
-      <c r="L6" s="39"/>
-      <c r="M6" s="39"/>
-      <c r="N6" s="39"/>
-      <c r="O6" s="39"/>
-      <c r="P6" s="39"/>
-      <c r="Q6" s="39"/>
-      <c r="R6" s="39"/>
-      <c r="S6" s="39"/>
-      <c r="T6" s="39"/>
-      <c r="U6" s="39"/>
-      <c r="V6" s="39"/>
-      <c r="W6" s="39"/>
-      <c r="X6" s="39"/>
-      <c r="Y6" s="39"/>
-      <c r="Z6" s="39"/>
-      <c r="AA6" s="39"/>
-      <c r="AB6" s="39"/>
-      <c r="AC6" s="39"/>
-      <c r="AD6" s="39"/>
-      <c r="AE6" s="39"/>
-      <c r="AF6" s="39"/>
-      <c r="AG6" s="39"/>
-      <c r="AH6" s="39"/>
-      <c r="AI6" s="39"/>
-      <c r="AJ6" s="39"/>
-      <c r="AK6" s="39"/>
-      <c r="AL6" s="39"/>
-      <c r="AM6" s="39"/>
-      <c r="AN6" s="39"/>
-      <c r="AO6" s="39"/>
-      <c r="AP6" s="39"/>
-      <c r="AQ6" s="39"/>
-      <c r="AR6" s="39"/>
-      <c r="AS6" s="39"/>
-      <c r="AT6" s="39"/>
-      <c r="AU6" s="39"/>
-      <c r="AV6" s="39"/>
-      <c r="AW6" s="39"/>
-      <c r="AX6" s="39"/>
-      <c r="AY6" s="39"/>
-      <c r="AZ6" s="39"/>
-      <c r="BA6" s="39"/>
-      <c r="BB6" s="39"/>
-      <c r="BC6" s="39"/>
-      <c r="BD6" s="39"/>
-      <c r="BE6" s="39"/>
-      <c r="BF6" s="39"/>
-      <c r="BG6" s="39"/>
-      <c r="BH6" s="39"/>
-      <c r="BI6" s="39"/>
-      <c r="BJ6" s="39"/>
-      <c r="BK6" s="39"/>
-      <c r="BL6" s="39"/>
-      <c r="BM6" s="39"/>
-      <c r="BN6" s="39"/>
-      <c r="BO6" s="39"/>
-      <c r="BP6" s="39"/>
-      <c r="BQ6" s="39"/>
-      <c r="BR6" s="39"/>
-      <c r="BS6" s="39"/>
-      <c r="BT6" s="39"/>
-      <c r="BU6" s="39"/>
-      <c r="BV6" s="39"/>
-      <c r="BW6" s="39"/>
-      <c r="BX6" s="39"/>
-      <c r="BY6" s="39"/>
-      <c r="BZ6" s="39"/>
-      <c r="CA6" s="39"/>
-      <c r="CB6" s="39"/>
-      <c r="CC6" s="39"/>
-      <c r="CD6" s="39"/>
-      <c r="CE6" s="39"/>
-      <c r="CF6" s="39"/>
-      <c r="CG6" s="39"/>
-      <c r="CH6" s="39"/>
-      <c r="CI6" s="39"/>
-      <c r="CJ6" s="40"/>
-    </row>
-    <row r="7" spans="1:88" s="18" customFormat="1" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="139" t="s">
-        <v>50</v>
-      </c>
-      <c r="B7" s="139" t="s">
-        <v>128</v>
-      </c>
-      <c r="C7" s="48"/>
-      <c r="D7" s="31"/>
+      <c r="C7" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="49" t="s">
+        <v>23</v>
+      </c>
       <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
       <c r="H7" s="39"/>
       <c r="I7" s="39"/>
       <c r="J7" s="39"/>
@@ -4427,15 +3933,11 @@
       <c r="CI7" s="39"/>
       <c r="CJ7" s="40"/>
     </row>
-    <row r="8" spans="1:88" s="18" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="55" t="s">
-        <v>130</v>
-      </c>
-      <c r="B8" s="124">
-        <v>9</v>
-      </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="10"/>
+    <row r="8" spans="1:88" s="18" customFormat="1" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="132"/>
+      <c r="B8" s="132"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="31"/>
       <c r="E8" s="39"/>
       <c r="F8" s="39"/>
       <c r="G8" s="39"/>
@@ -4522,12 +4024,8 @@
       <c r="CJ8" s="40"/>
     </row>
     <row r="9" spans="1:88" s="18" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="55" t="s">
-        <v>129</v>
-      </c>
-      <c r="B9" s="124">
-        <v>11</v>
-      </c>
+      <c r="A9" s="55"/>
+      <c r="B9" s="117"/>
       <c r="C9" s="9"/>
       <c r="D9" s="10"/>
       <c r="E9" s="39"/>
@@ -4616,14 +4114,10 @@
       <c r="CJ9" s="40"/>
     </row>
     <row r="10" spans="1:88" s="18" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="124" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" s="125" t="s">
-        <v>116</v>
-      </c>
-      <c r="C10" s="26"/>
-      <c r="D10" s="144"/>
+      <c r="A10" s="55"/>
+      <c r="B10" s="117"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="10"/>
       <c r="E10" s="39"/>
       <c r="F10" s="39"/>
       <c r="G10" s="39"/>
@@ -4710,14 +4204,10 @@
       <c r="CJ10" s="40"/>
     </row>
     <row r="11" spans="1:88" s="18" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="140" t="s">
-        <v>56</v>
-      </c>
-      <c r="B11" s="128" t="s">
-        <v>81</v>
-      </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="10"/>
+      <c r="A11" s="117"/>
+      <c r="B11" s="118"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="137"/>
       <c r="E11" s="39"/>
       <c r="F11" s="39"/>
       <c r="G11" s="39"/>
@@ -4804,14 +4294,10 @@
       <c r="CJ11" s="40"/>
     </row>
     <row r="12" spans="1:88" s="18" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="105" t="s">
-        <v>101</v>
-      </c>
-      <c r="B12" s="128">
-        <v>93</v>
-      </c>
-      <c r="C12" s="143"/>
-      <c r="D12" s="8"/>
+      <c r="A12" s="133"/>
+      <c r="B12" s="121"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="10"/>
       <c r="E12" s="39"/>
       <c r="F12" s="39"/>
       <c r="G12" s="39"/>
@@ -4898,14 +4384,10 @@
       <c r="CJ12" s="40"/>
     </row>
     <row r="13" spans="1:88" s="18" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="105" t="s">
-        <v>53</v>
-      </c>
-      <c r="B13" s="124" t="s">
-        <v>117</v>
-      </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="46"/>
+      <c r="A13" s="101"/>
+      <c r="B13" s="121"/>
+      <c r="C13" s="136"/>
+      <c r="D13" s="8"/>
       <c r="E13" s="39"/>
       <c r="F13" s="39"/>
       <c r="G13" s="39"/>
@@ -4992,17 +4474,13 @@
       <c r="CJ13" s="40"/>
     </row>
     <row r="14" spans="1:88" s="18" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="105" t="s">
-        <v>55</v>
-      </c>
-      <c r="B14" s="124" t="s">
-        <v>131</v>
-      </c>
+      <c r="A14" s="101"/>
+      <c r="B14" s="117"/>
       <c r="C14" s="17"/>
-      <c r="D14" s="16"/>
+      <c r="D14" s="46"/>
       <c r="E14" s="39"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="41"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
       <c r="H14" s="39"/>
       <c r="I14" s="39"/>
       <c r="J14" s="39"/>
@@ -5086,14 +4564,10 @@
       <c r="CJ14" s="40"/>
     </row>
     <row r="15" spans="1:88" s="18" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="55" t="s">
-        <v>52</v>
-      </c>
-      <c r="B15" s="127" t="s">
-        <v>80</v>
-      </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="45"/>
+      <c r="A15" s="101"/>
+      <c r="B15" s="117"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="16"/>
       <c r="E15" s="39"/>
       <c r="F15" s="41"/>
       <c r="G15" s="41"/>
@@ -5180,17 +4654,13 @@
       <c r="CJ15" s="40"/>
     </row>
     <row r="16" spans="1:88" s="18" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="105" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" s="142" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" s="17"/>
-      <c r="D16" s="10"/>
+      <c r="A16" s="55"/>
+      <c r="B16" s="120"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="45"/>
       <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
       <c r="H16" s="39"/>
       <c r="I16" s="39"/>
       <c r="J16" s="39"/>
@@ -5273,109 +4743,101 @@
       <c r="CI16" s="39"/>
       <c r="CJ16" s="40"/>
     </row>
-    <row r="17" spans="1:88" s="43" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="104" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="141" t="s">
-        <v>98</v>
-      </c>
-      <c r="C17" s="143"/>
+    <row r="17" spans="1:88" s="18" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="101"/>
+      <c r="B17" s="135"/>
+      <c r="C17" s="17"/>
       <c r="D17" s="10"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
-      <c r="K17" s="42"/>
-      <c r="L17" s="42"/>
-      <c r="M17" s="42"/>
-      <c r="N17" s="42"/>
-      <c r="O17" s="42"/>
-      <c r="P17" s="42"/>
-      <c r="Q17" s="42"/>
-      <c r="R17" s="42"/>
-      <c r="S17" s="42"/>
-      <c r="T17" s="42"/>
-      <c r="U17" s="42"/>
-      <c r="V17" s="42"/>
-      <c r="W17" s="42"/>
-      <c r="X17" s="42"/>
-      <c r="Y17" s="42"/>
-      <c r="Z17" s="42"/>
-      <c r="AA17" s="42"/>
-      <c r="AB17" s="42"/>
-      <c r="AC17" s="42"/>
-      <c r="AD17" s="42"/>
-      <c r="AE17" s="42"/>
-      <c r="AF17" s="42"/>
-      <c r="AG17" s="42"/>
-      <c r="AH17" s="42"/>
-      <c r="AI17" s="42"/>
-      <c r="AJ17" s="42"/>
-      <c r="AK17" s="42"/>
-      <c r="AL17" s="42"/>
-      <c r="AM17" s="42"/>
-      <c r="AN17" s="42"/>
-      <c r="AO17" s="42"/>
-      <c r="AP17" s="42"/>
-      <c r="AQ17" s="42"/>
-      <c r="AR17" s="42"/>
-      <c r="AS17" s="42"/>
-      <c r="AT17" s="42"/>
-      <c r="AU17" s="42"/>
-      <c r="AV17" s="42"/>
-      <c r="AW17" s="42"/>
-      <c r="AX17" s="42"/>
-      <c r="AY17" s="42"/>
-      <c r="AZ17" s="42"/>
-      <c r="BA17" s="42"/>
-      <c r="BB17" s="42"/>
-      <c r="BC17" s="42"/>
-      <c r="BD17" s="42"/>
-      <c r="BE17" s="42"/>
-      <c r="BF17" s="42"/>
-      <c r="BG17" s="42"/>
-      <c r="BH17" s="42"/>
-      <c r="BI17" s="42"/>
-      <c r="BJ17" s="42"/>
-      <c r="BK17" s="42"/>
-      <c r="BL17" s="42"/>
-      <c r="BM17" s="42"/>
-      <c r="BN17" s="42"/>
-      <c r="BO17" s="42"/>
-      <c r="BP17" s="42"/>
-      <c r="BQ17" s="42"/>
-      <c r="BR17" s="42"/>
-      <c r="BS17" s="42"/>
-      <c r="BT17" s="42"/>
-      <c r="BU17" s="42"/>
-      <c r="BV17" s="42"/>
-      <c r="BW17" s="42"/>
-      <c r="BX17" s="42"/>
-      <c r="BY17" s="42"/>
-      <c r="BZ17" s="42"/>
-      <c r="CA17" s="42"/>
-      <c r="CB17" s="42"/>
-      <c r="CC17" s="42"/>
-      <c r="CD17" s="42"/>
-      <c r="CE17" s="42"/>
-      <c r="CF17" s="42"/>
-      <c r="CG17" s="42"/>
-      <c r="CH17" s="42"/>
-      <c r="CI17" s="42"/>
-      <c r="CJ17" s="44"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="39"/>
+      <c r="I17" s="39"/>
+      <c r="J17" s="39"/>
+      <c r="K17" s="39"/>
+      <c r="L17" s="39"/>
+      <c r="M17" s="39"/>
+      <c r="N17" s="39"/>
+      <c r="O17" s="39"/>
+      <c r="P17" s="39"/>
+      <c r="Q17" s="39"/>
+      <c r="R17" s="39"/>
+      <c r="S17" s="39"/>
+      <c r="T17" s="39"/>
+      <c r="U17" s="39"/>
+      <c r="V17" s="39"/>
+      <c r="W17" s="39"/>
+      <c r="X17" s="39"/>
+      <c r="Y17" s="39"/>
+      <c r="Z17" s="39"/>
+      <c r="AA17" s="39"/>
+      <c r="AB17" s="39"/>
+      <c r="AC17" s="39"/>
+      <c r="AD17" s="39"/>
+      <c r="AE17" s="39"/>
+      <c r="AF17" s="39"/>
+      <c r="AG17" s="39"/>
+      <c r="AH17" s="39"/>
+      <c r="AI17" s="39"/>
+      <c r="AJ17" s="39"/>
+      <c r="AK17" s="39"/>
+      <c r="AL17" s="39"/>
+      <c r="AM17" s="39"/>
+      <c r="AN17" s="39"/>
+      <c r="AO17" s="39"/>
+      <c r="AP17" s="39"/>
+      <c r="AQ17" s="39"/>
+      <c r="AR17" s="39"/>
+      <c r="AS17" s="39"/>
+      <c r="AT17" s="39"/>
+      <c r="AU17" s="39"/>
+      <c r="AV17" s="39"/>
+      <c r="AW17" s="39"/>
+      <c r="AX17" s="39"/>
+      <c r="AY17" s="39"/>
+      <c r="AZ17" s="39"/>
+      <c r="BA17" s="39"/>
+      <c r="BB17" s="39"/>
+      <c r="BC17" s="39"/>
+      <c r="BD17" s="39"/>
+      <c r="BE17" s="39"/>
+      <c r="BF17" s="39"/>
+      <c r="BG17" s="39"/>
+      <c r="BH17" s="39"/>
+      <c r="BI17" s="39"/>
+      <c r="BJ17" s="39"/>
+      <c r="BK17" s="39"/>
+      <c r="BL17" s="39"/>
+      <c r="BM17" s="39"/>
+      <c r="BN17" s="39"/>
+      <c r="BO17" s="39"/>
+      <c r="BP17" s="39"/>
+      <c r="BQ17" s="39"/>
+      <c r="BR17" s="39"/>
+      <c r="BS17" s="39"/>
+      <c r="BT17" s="39"/>
+      <c r="BU17" s="39"/>
+      <c r="BV17" s="39"/>
+      <c r="BW17" s="39"/>
+      <c r="BX17" s="39"/>
+      <c r="BY17" s="39"/>
+      <c r="BZ17" s="39"/>
+      <c r="CA17" s="39"/>
+      <c r="CB17" s="39"/>
+      <c r="CC17" s="39"/>
+      <c r="CD17" s="39"/>
+      <c r="CE17" s="39"/>
+      <c r="CF17" s="39"/>
+      <c r="CG17" s="39"/>
+      <c r="CH17" s="39"/>
+      <c r="CI17" s="39"/>
+      <c r="CJ17" s="40"/>
     </row>
     <row r="18" spans="1:88" s="43" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="105" t="s">
-        <v>57</v>
-      </c>
-      <c r="B18" s="126" t="s">
-        <v>79</v>
-      </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="8"/>
+      <c r="A18" s="100"/>
+      <c r="B18" s="134"/>
+      <c r="C18" s="136"/>
+      <c r="D18" s="10"/>
       <c r="E18" s="42"/>
       <c r="F18" s="42"/>
       <c r="G18" s="42"/>
@@ -5461,108 +4923,192 @@
       <c r="CI18" s="42"/>
       <c r="CJ18" s="44"/>
     </row>
-    <row r="19" spans="1:88" s="18" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="105" t="s">
-        <v>54</v>
-      </c>
-      <c r="B19" s="124" t="s">
-        <v>118</v>
-      </c>
-      <c r="C19" s="15"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="39"/>
-      <c r="I19" s="39"/>
-      <c r="J19" s="39"/>
-      <c r="K19" s="39"/>
-      <c r="L19" s="39"/>
-      <c r="M19" s="39"/>
-      <c r="N19" s="39"/>
-      <c r="O19" s="39"/>
-      <c r="P19" s="39"/>
-      <c r="Q19" s="39"/>
-      <c r="R19" s="39"/>
-      <c r="S19" s="39"/>
-      <c r="T19" s="39"/>
-      <c r="U19" s="39"/>
-      <c r="V19" s="39"/>
-      <c r="W19" s="39"/>
-      <c r="X19" s="39"/>
-      <c r="Y19" s="39"/>
-      <c r="Z19" s="39"/>
-      <c r="AA19" s="39"/>
-      <c r="AB19" s="39"/>
-      <c r="AC19" s="39"/>
-      <c r="AD19" s="39"/>
-      <c r="AE19" s="39"/>
-      <c r="AF19" s="39"/>
-      <c r="AG19" s="39"/>
-      <c r="AH19" s="39"/>
-      <c r="AI19" s="39"/>
-      <c r="AJ19" s="39"/>
-      <c r="AK19" s="39"/>
-      <c r="AL19" s="39"/>
-      <c r="AM19" s="39"/>
-      <c r="AN19" s="39"/>
-      <c r="AO19" s="39"/>
-      <c r="AP19" s="39"/>
-      <c r="AQ19" s="39"/>
-      <c r="AR19" s="39"/>
-      <c r="AS19" s="39"/>
-      <c r="AT19" s="39"/>
-      <c r="AU19" s="39"/>
-      <c r="AV19" s="39"/>
-      <c r="AW19" s="39"/>
-      <c r="AX19" s="39"/>
-      <c r="AY19" s="39"/>
-      <c r="AZ19" s="39"/>
-      <c r="BA19" s="39"/>
-      <c r="BB19" s="39"/>
-      <c r="BC19" s="39"/>
-      <c r="BD19" s="39"/>
-      <c r="BE19" s="39"/>
-      <c r="BF19" s="39"/>
-      <c r="BG19" s="39"/>
-      <c r="BH19" s="39"/>
-      <c r="BI19" s="39"/>
-      <c r="BJ19" s="39"/>
-      <c r="BK19" s="39"/>
-      <c r="BL19" s="39"/>
-      <c r="BM19" s="39"/>
-      <c r="BN19" s="39"/>
-      <c r="BO19" s="39"/>
-      <c r="BP19" s="39"/>
-      <c r="BQ19" s="39"/>
-      <c r="BR19" s="39"/>
-      <c r="BS19" s="39"/>
-      <c r="BT19" s="39"/>
-      <c r="BU19" s="39"/>
-      <c r="BV19" s="39"/>
-      <c r="BW19" s="39"/>
-      <c r="BX19" s="39"/>
-      <c r="BY19" s="39"/>
-      <c r="BZ19" s="39"/>
-      <c r="CA19" s="39"/>
-      <c r="CB19" s="39"/>
-      <c r="CC19" s="39"/>
-      <c r="CD19" s="39"/>
-      <c r="CE19" s="39"/>
-      <c r="CF19" s="39"/>
-      <c r="CG19" s="39"/>
-      <c r="CH19" s="39"/>
-      <c r="CI19" s="39"/>
-      <c r="CJ19" s="40"/>
+    <row r="19" spans="1:88" s="43" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="101"/>
+      <c r="B19" s="119"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="42"/>
+      <c r="H19" s="42"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
+      <c r="K19" s="42"/>
+      <c r="L19" s="42"/>
+      <c r="M19" s="42"/>
+      <c r="N19" s="42"/>
+      <c r="O19" s="42"/>
+      <c r="P19" s="42"/>
+      <c r="Q19" s="42"/>
+      <c r="R19" s="42"/>
+      <c r="S19" s="42"/>
+      <c r="T19" s="42"/>
+      <c r="U19" s="42"/>
+      <c r="V19" s="42"/>
+      <c r="W19" s="42"/>
+      <c r="X19" s="42"/>
+      <c r="Y19" s="42"/>
+      <c r="Z19" s="42"/>
+      <c r="AA19" s="42"/>
+      <c r="AB19" s="42"/>
+      <c r="AC19" s="42"/>
+      <c r="AD19" s="42"/>
+      <c r="AE19" s="42"/>
+      <c r="AF19" s="42"/>
+      <c r="AG19" s="42"/>
+      <c r="AH19" s="42"/>
+      <c r="AI19" s="42"/>
+      <c r="AJ19" s="42"/>
+      <c r="AK19" s="42"/>
+      <c r="AL19" s="42"/>
+      <c r="AM19" s="42"/>
+      <c r="AN19" s="42"/>
+      <c r="AO19" s="42"/>
+      <c r="AP19" s="42"/>
+      <c r="AQ19" s="42"/>
+      <c r="AR19" s="42"/>
+      <c r="AS19" s="42"/>
+      <c r="AT19" s="42"/>
+      <c r="AU19" s="42"/>
+      <c r="AV19" s="42"/>
+      <c r="AW19" s="42"/>
+      <c r="AX19" s="42"/>
+      <c r="AY19" s="42"/>
+      <c r="AZ19" s="42"/>
+      <c r="BA19" s="42"/>
+      <c r="BB19" s="42"/>
+      <c r="BC19" s="42"/>
+      <c r="BD19" s="42"/>
+      <c r="BE19" s="42"/>
+      <c r="BF19" s="42"/>
+      <c r="BG19" s="42"/>
+      <c r="BH19" s="42"/>
+      <c r="BI19" s="42"/>
+      <c r="BJ19" s="42"/>
+      <c r="BK19" s="42"/>
+      <c r="BL19" s="42"/>
+      <c r="BM19" s="42"/>
+      <c r="BN19" s="42"/>
+      <c r="BO19" s="42"/>
+      <c r="BP19" s="42"/>
+      <c r="BQ19" s="42"/>
+      <c r="BR19" s="42"/>
+      <c r="BS19" s="42"/>
+      <c r="BT19" s="42"/>
+      <c r="BU19" s="42"/>
+      <c r="BV19" s="42"/>
+      <c r="BW19" s="42"/>
+      <c r="BX19" s="42"/>
+      <c r="BY19" s="42"/>
+      <c r="BZ19" s="42"/>
+      <c r="CA19" s="42"/>
+      <c r="CB19" s="42"/>
+      <c r="CC19" s="42"/>
+      <c r="CD19" s="42"/>
+      <c r="CE19" s="42"/>
+      <c r="CF19" s="42"/>
+      <c r="CG19" s="42"/>
+      <c r="CH19" s="42"/>
+      <c r="CI19" s="42"/>
+      <c r="CJ19" s="44"/>
+    </row>
+    <row r="20" spans="1:88" s="18" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="101"/>
+      <c r="B20" s="117"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="39"/>
+      <c r="F20" s="39"/>
+      <c r="G20" s="39"/>
+      <c r="H20" s="39"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
+      <c r="K20" s="39"/>
+      <c r="L20" s="39"/>
+      <c r="M20" s="39"/>
+      <c r="N20" s="39"/>
+      <c r="O20" s="39"/>
+      <c r="P20" s="39"/>
+      <c r="Q20" s="39"/>
+      <c r="R20" s="39"/>
+      <c r="S20" s="39"/>
+      <c r="T20" s="39"/>
+      <c r="U20" s="39"/>
+      <c r="V20" s="39"/>
+      <c r="W20" s="39"/>
+      <c r="X20" s="39"/>
+      <c r="Y20" s="39"/>
+      <c r="Z20" s="39"/>
+      <c r="AA20" s="39"/>
+      <c r="AB20" s="39"/>
+      <c r="AC20" s="39"/>
+      <c r="AD20" s="39"/>
+      <c r="AE20" s="39"/>
+      <c r="AF20" s="39"/>
+      <c r="AG20" s="39"/>
+      <c r="AH20" s="39"/>
+      <c r="AI20" s="39"/>
+      <c r="AJ20" s="39"/>
+      <c r="AK20" s="39"/>
+      <c r="AL20" s="39"/>
+      <c r="AM20" s="39"/>
+      <c r="AN20" s="39"/>
+      <c r="AO20" s="39"/>
+      <c r="AP20" s="39"/>
+      <c r="AQ20" s="39"/>
+      <c r="AR20" s="39"/>
+      <c r="AS20" s="39"/>
+      <c r="AT20" s="39"/>
+      <c r="AU20" s="39"/>
+      <c r="AV20" s="39"/>
+      <c r="AW20" s="39"/>
+      <c r="AX20" s="39"/>
+      <c r="AY20" s="39"/>
+      <c r="AZ20" s="39"/>
+      <c r="BA20" s="39"/>
+      <c r="BB20" s="39"/>
+      <c r="BC20" s="39"/>
+      <c r="BD20" s="39"/>
+      <c r="BE20" s="39"/>
+      <c r="BF20" s="39"/>
+      <c r="BG20" s="39"/>
+      <c r="BH20" s="39"/>
+      <c r="BI20" s="39"/>
+      <c r="BJ20" s="39"/>
+      <c r="BK20" s="39"/>
+      <c r="BL20" s="39"/>
+      <c r="BM20" s="39"/>
+      <c r="BN20" s="39"/>
+      <c r="BO20" s="39"/>
+      <c r="BP20" s="39"/>
+      <c r="BQ20" s="39"/>
+      <c r="BR20" s="39"/>
+      <c r="BS20" s="39"/>
+      <c r="BT20" s="39"/>
+      <c r="BU20" s="39"/>
+      <c r="BV20" s="39"/>
+      <c r="BW20" s="39"/>
+      <c r="BX20" s="39"/>
+      <c r="BY20" s="39"/>
+      <c r="BZ20" s="39"/>
+      <c r="CA20" s="39"/>
+      <c r="CB20" s="39"/>
+      <c r="CC20" s="39"/>
+      <c r="CD20" s="39"/>
+      <c r="CE20" s="39"/>
+      <c r="CF20" s="39"/>
+      <c r="CG20" s="39"/>
+      <c r="CH20" s="39"/>
+      <c r="CI20" s="39"/>
+      <c r="CJ20" s="40"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
+  <mergeCells count="1">
+    <mergeCell ref="F6:G6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="82" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="22" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <tableParts count="1">
     <tablePart r:id="rId3"/>
@@ -5590,12 +5136,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="183" t="s">
-        <v>77</v>
-      </c>
-      <c r="B1" s="183"/>
-      <c r="C1" s="183"/>
-      <c r="D1" s="183"/>
+      <c r="A1" s="174" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="174"/>
+      <c r="C1" s="174"/>
+      <c r="D1" s="174"/>
       <c r="E1" s="25"/>
       <c r="F1" s="25"/>
       <c r="G1" s="25"/>
@@ -5606,7 +5152,7 @@
       <c r="A2" s="31"/>
       <c r="B2" s="31"/>
       <c r="C2" s="33" t="s">
-        <v>58</v>
+        <v>7</v>
       </c>
       <c r="D2" s="25"/>
       <c r="E2" s="25"/>
@@ -5616,10 +5162,10 @@
       <c r="I2" s="25"/>
     </row>
     <row r="3" spans="1:9" ht="21" x14ac:dyDescent="0.2">
-      <c r="A3" s="184"/>
-      <c r="B3" s="184"/>
-      <c r="C3" s="184"/>
-      <c r="D3" s="184"/>
+      <c r="A3" s="175"/>
+      <c r="B3" s="175"/>
+      <c r="C3" s="175"/>
+      <c r="D3" s="175"/>
       <c r="E3" s="25"/>
       <c r="F3" s="25"/>
       <c r="G3" s="25"/>
@@ -5645,10 +5191,10 @@
         <v>0</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>75</v>
+        <v>24</v>
       </c>
       <c r="D5" s="59" t="s">
-        <v>74</v>
+        <v>23</v>
       </c>
       <c r="E5" s="25"/>
       <c r="F5" s="25"/>
@@ -5657,11 +5203,11 @@
       <c r="I5" s="25"/>
     </row>
     <row r="6" spans="1:9" ht="57.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="129" t="s">
-        <v>73</v>
-      </c>
-      <c r="B6" s="135" t="s">
-        <v>132</v>
+      <c r="A6" s="122" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="128" t="s">
+        <v>38</v>
       </c>
       <c r="C6" s="29"/>
       <c r="D6" s="56"/>
@@ -5672,11 +5218,11 @@
       <c r="I6" s="25"/>
     </row>
     <row r="7" spans="1:9" ht="57.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="131" t="s">
-        <v>71</v>
-      </c>
-      <c r="B7" s="132" t="s">
-        <v>84</v>
+      <c r="A7" s="124" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="125" t="s">
+        <v>30</v>
       </c>
       <c r="C7" s="24"/>
       <c r="D7" s="25"/>
@@ -5687,11 +5233,11 @@
       <c r="I7" s="25"/>
     </row>
     <row r="8" spans="1:9" ht="57.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="131" t="s">
-        <v>61</v>
-      </c>
-      <c r="B8" s="133" t="s">
-        <v>60</v>
+      <c r="A8" s="124" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="126" t="s">
+        <v>9</v>
       </c>
       <c r="C8" s="24"/>
       <c r="D8" s="62"/>
@@ -5702,11 +5248,11 @@
       <c r="I8" s="25"/>
     </row>
     <row r="9" spans="1:9" ht="57.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="131" t="s">
-        <v>70</v>
-      </c>
-      <c r="B9" s="134" t="s">
-        <v>69</v>
+      <c r="A9" s="124" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="127" t="s">
+        <v>18</v>
       </c>
       <c r="C9" s="24"/>
       <c r="D9" s="56"/>
@@ -5717,11 +5263,11 @@
       <c r="I9" s="25"/>
     </row>
     <row r="10" spans="1:9" ht="57.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="129" t="s">
-        <v>68</v>
-      </c>
-      <c r="B10" s="130" t="s">
-        <v>82</v>
+      <c r="A10" s="122" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="123" t="s">
+        <v>28</v>
       </c>
       <c r="C10" s="29"/>
       <c r="D10" s="56"/>
@@ -5732,11 +5278,11 @@
       <c r="I10" s="25"/>
     </row>
     <row r="11" spans="1:9" ht="57.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="129" t="s">
-        <v>67</v>
-      </c>
-      <c r="B11" s="130" t="s">
-        <v>85</v>
+      <c r="A11" s="122" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="123" t="s">
+        <v>31</v>
       </c>
       <c r="C11" s="29"/>
       <c r="D11" s="56"/>
@@ -5747,11 +5293,11 @@
       <c r="I11" s="25"/>
     </row>
     <row r="12" spans="1:9" ht="57.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="129" t="s">
-        <v>72</v>
-      </c>
-      <c r="B12" s="130" t="s">
-        <v>27</v>
+      <c r="A12" s="122" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="123" t="s">
+        <v>2</v>
       </c>
       <c r="C12" s="29"/>
       <c r="D12" s="56"/>
@@ -5762,11 +5308,11 @@
       <c r="I12" s="25"/>
     </row>
     <row r="13" spans="1:9" ht="57.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="129" t="s">
-        <v>64</v>
-      </c>
-      <c r="B13" s="130" t="s">
-        <v>83</v>
+      <c r="A13" s="122" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="123" t="s">
+        <v>29</v>
       </c>
       <c r="C13" s="29"/>
       <c r="D13" s="56"/>
@@ -5777,11 +5323,11 @@
       <c r="I13" s="25"/>
     </row>
     <row r="14" spans="1:9" ht="57.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="129" t="s">
-        <v>63</v>
-      </c>
-      <c r="B14" s="135" t="s">
-        <v>119</v>
+      <c r="A14" s="122" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="128" t="s">
+        <v>37</v>
       </c>
       <c r="C14" s="29"/>
       <c r="D14" s="56"/>
@@ -5792,10 +5338,10 @@
       <c r="I14" s="25"/>
     </row>
     <row r="15" spans="1:9" ht="57.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="131" t="s">
-        <v>104</v>
-      </c>
-      <c r="B15" s="132">
+      <c r="A15" s="124" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="125">
         <v>58</v>
       </c>
       <c r="C15" s="24"/>
@@ -5808,10 +5354,10 @@
     </row>
     <row r="16" spans="1:9" ht="57.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="51" t="s">
-        <v>65</v>
-      </c>
-      <c r="B16" s="130" t="s">
-        <v>86</v>
+        <v>14</v>
+      </c>
+      <c r="B16" s="123" t="s">
+        <v>32</v>
       </c>
       <c r="C16" s="29"/>
       <c r="D16" s="56"/>
@@ -5822,10 +5368,10 @@
       <c r="I16" s="25"/>
     </row>
     <row r="17" spans="1:9" ht="57.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="104" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="176">
+      <c r="A17" s="100" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="168">
         <v>61</v>
       </c>
       <c r="C17" s="24"/>
@@ -5837,11 +5383,11 @@
       <c r="I17" s="25"/>
     </row>
     <row r="18" spans="1:9" ht="57.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="129" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" s="130" t="s">
-        <v>133</v>
+      <c r="A18" s="122" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="123" t="s">
+        <v>39</v>
       </c>
       <c r="C18" s="29"/>
       <c r="D18" s="56"/>
@@ -5852,11 +5398,11 @@
       <c r="I18" s="25"/>
     </row>
     <row r="19" spans="1:9" ht="57.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="129" t="s">
-        <v>59</v>
-      </c>
-      <c r="B19" s="130" t="s">
-        <v>111</v>
+      <c r="A19" s="122" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="123" t="s">
+        <v>35</v>
       </c>
       <c r="C19" s="24"/>
       <c r="D19" s="56"/>
@@ -5867,11 +5413,11 @@
       <c r="I19" s="25"/>
     </row>
     <row r="20" spans="1:9" ht="57.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="129" t="s">
-        <v>66</v>
-      </c>
-      <c r="B20" s="130" t="s">
-        <v>36</v>
+      <c r="A20" s="122" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="123" t="s">
+        <v>3</v>
       </c>
       <c r="C20" s="29"/>
       <c r="D20" s="56"/>
@@ -5882,11 +5428,11 @@
       <c r="I20" s="25"/>
     </row>
     <row r="21" spans="1:9" ht="57.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="129" t="s">
-        <v>54</v>
-      </c>
-      <c r="B21" s="130" t="s">
-        <v>134</v>
+      <c r="A21" s="122" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="123" t="s">
+        <v>40</v>
       </c>
       <c r="C21" s="70"/>
       <c r="D21" s="56"/>
@@ -5897,11 +5443,11 @@
       <c r="I21" s="25"/>
     </row>
     <row r="22" spans="1:9" ht="57.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="136" t="s">
-        <v>62</v>
-      </c>
-      <c r="B22" s="137" t="s">
-        <v>112</v>
+      <c r="A22" s="129" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="130" t="s">
+        <v>36</v>
       </c>
       <c r="C22" s="71"/>
       <c r="D22" s="60"/>
@@ -5944,8 +5490,8 @@
   </sheetPr>
   <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A37" zoomScale="60" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5957,7 +5503,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="92" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B1" s="67" t="s">
-        <v>100</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.25">
@@ -5965,464 +5511,334 @@
         <v>1</v>
       </c>
       <c r="B3" s="50" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="C3" s="59" t="s">
-        <v>74</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="147" t="s">
-        <v>30</v>
-      </c>
+      <c r="A4" s="140"/>
       <c r="B4" s="61"/>
       <c r="C4" s="56"/>
     </row>
     <row r="5" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="145" t="s">
-        <v>50</v>
-      </c>
+      <c r="A5" s="138"/>
       <c r="B5" s="61"/>
       <c r="C5" s="56"/>
     </row>
     <row r="6" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="149" t="s">
-        <v>107</v>
-      </c>
+      <c r="A6" s="142"/>
       <c r="B6" s="61"/>
       <c r="C6" s="56"/>
     </row>
     <row r="7" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="161" t="s">
-        <v>130</v>
-      </c>
+      <c r="A7" s="154"/>
       <c r="B7" s="61"/>
       <c r="C7" s="56"/>
     </row>
     <row r="8" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="155" t="s">
-        <v>29</v>
-      </c>
+      <c r="A8" s="148"/>
       <c r="B8" s="61"/>
       <c r="C8" s="56"/>
     </row>
     <row r="9" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="147" t="s">
-        <v>14</v>
-      </c>
+      <c r="A9" s="140"/>
       <c r="B9" s="61"/>
       <c r="C9" s="56"/>
     </row>
     <row r="10" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="148" t="s">
-        <v>21</v>
-      </c>
+      <c r="A10" s="141"/>
       <c r="B10" s="61"/>
       <c r="C10" s="56"/>
     </row>
     <row r="11" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="146" t="s">
-        <v>73</v>
-      </c>
+      <c r="A11" s="139"/>
       <c r="B11" s="61"/>
       <c r="C11" s="56"/>
     </row>
     <row r="12" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="147" t="s">
-        <v>22</v>
-      </c>
+      <c r="A12" s="140"/>
       <c r="B12" s="61"/>
       <c r="C12" s="60"/>
     </row>
     <row r="13" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="52" t="s">
-        <v>124</v>
-      </c>
+      <c r="A13" s="52"/>
       <c r="B13" s="64"/>
       <c r="C13" s="56"/>
     </row>
     <row r="14" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="171" t="s">
-        <v>26</v>
-      </c>
+      <c r="A14" s="164"/>
       <c r="B14" s="65"/>
       <c r="C14" s="56"/>
     </row>
     <row r="15" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="149" t="s">
-        <v>6</v>
-      </c>
+      <c r="A15" s="142"/>
       <c r="B15" s="64"/>
       <c r="C15" s="56"/>
     </row>
     <row r="16" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="165" t="s">
-        <v>37</v>
-      </c>
+      <c r="A16" s="158"/>
       <c r="B16" s="65"/>
       <c r="C16" s="56"/>
     </row>
     <row r="17" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="148" t="s">
-        <v>71</v>
-      </c>
+      <c r="A17" s="141"/>
       <c r="B17" s="64"/>
       <c r="C17" s="56"/>
     </row>
     <row r="18" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="149" t="s">
-        <v>3</v>
-      </c>
+      <c r="A18" s="142"/>
       <c r="B18" s="64"/>
       <c r="C18" s="56"/>
     </row>
     <row r="19" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="151" t="s">
-        <v>15</v>
-      </c>
+      <c r="A19" s="144"/>
       <c r="B19" s="64"/>
       <c r="C19" s="56"/>
     </row>
     <row r="20" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="149" t="s">
-        <v>129</v>
-      </c>
+      <c r="A20" s="142"/>
       <c r="B20" s="64"/>
       <c r="C20" s="56"/>
     </row>
     <row r="21" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="149" t="s">
-        <v>4</v>
-      </c>
+      <c r="A21" s="142"/>
       <c r="B21" s="64"/>
       <c r="C21" s="56"/>
     </row>
     <row r="22" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="148" t="s">
-        <v>51</v>
-      </c>
+      <c r="A22" s="141"/>
       <c r="B22" s="64"/>
       <c r="C22" s="56"/>
     </row>
     <row r="23" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="173" t="s">
-        <v>19</v>
-      </c>
+      <c r="A23" s="166"/>
       <c r="B23" s="64"/>
       <c r="C23" s="56"/>
     </row>
     <row r="24" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="104" t="s">
-        <v>56</v>
-      </c>
+      <c r="A24" s="100"/>
       <c r="B24" s="64"/>
       <c r="C24" s="56"/>
     </row>
     <row r="25" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="164" t="s">
-        <v>121</v>
-      </c>
+      <c r="A25" s="157"/>
       <c r="B25" s="64"/>
       <c r="C25" s="56"/>
     </row>
     <row r="26" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="148" t="s">
-        <v>61</v>
-      </c>
+      <c r="A26" s="141"/>
       <c r="B26" s="64"/>
       <c r="C26" s="56"/>
     </row>
     <row r="27" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="157" t="s">
-        <v>49</v>
-      </c>
+      <c r="A27" s="150"/>
       <c r="B27" s="64"/>
       <c r="C27" s="56"/>
     </row>
     <row r="28" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="151" t="s">
-        <v>24</v>
-      </c>
+      <c r="A28" s="144"/>
       <c r="B28" s="64"/>
       <c r="C28" s="56"/>
     </row>
     <row r="29" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="147" t="s">
-        <v>101</v>
-      </c>
+      <c r="A29" s="140"/>
       <c r="B29" s="64"/>
       <c r="C29" s="56"/>
     </row>
     <row r="30" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="149" t="s">
-        <v>96</v>
-      </c>
+      <c r="A30" s="142"/>
       <c r="B30" s="64"/>
       <c r="C30" s="56"/>
     </row>
     <row r="31" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="150" t="s">
-        <v>53</v>
-      </c>
+      <c r="A31" s="143"/>
       <c r="B31" s="64"/>
       <c r="C31" s="56"/>
     </row>
     <row r="32" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="164" t="s">
-        <v>122</v>
-      </c>
+      <c r="A32" s="157"/>
       <c r="B32" s="64"/>
       <c r="C32" s="56"/>
     </row>
     <row r="33" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="148" t="s">
-        <v>70</v>
-      </c>
+      <c r="A33" s="141"/>
       <c r="B33" s="64"/>
       <c r="C33" s="56"/>
     </row>
     <row r="34" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="166" t="s">
-        <v>68</v>
-      </c>
+      <c r="A34" s="159"/>
       <c r="B34" s="64"/>
       <c r="C34" s="56"/>
     </row>
     <row r="35" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="149" t="s">
-        <v>12</v>
-      </c>
+      <c r="A35" s="142"/>
       <c r="B35" s="64"/>
       <c r="C35" s="56"/>
     </row>
     <row r="36" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="147" t="s">
-        <v>55</v>
-      </c>
+      <c r="A36" s="140"/>
       <c r="B36" s="66"/>
       <c r="C36" s="56"/>
     </row>
     <row r="37" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="145" t="s">
-        <v>103</v>
-      </c>
+      <c r="A37" s="138"/>
       <c r="B37" s="64"/>
       <c r="C37" s="56"/>
     </row>
     <row r="38" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="145" t="s">
-        <v>67</v>
-      </c>
+      <c r="A38" s="138"/>
       <c r="B38" s="64"/>
       <c r="C38" s="56"/>
     </row>
     <row r="39" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="156" t="s">
-        <v>42</v>
-      </c>
+      <c r="A39" s="149"/>
       <c r="B39" s="64"/>
       <c r="C39" s="56"/>
     </row>
-    <row r="40" spans="1:3" s="169" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="63" t="s">
-        <v>17</v>
-      </c>
-      <c r="B40" s="167"/>
-      <c r="C40" s="168"/>
+    <row r="40" spans="1:3" s="162" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="63"/>
+      <c r="B40" s="160"/>
+      <c r="C40" s="161"/>
     </row>
     <row r="41" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="145" t="s">
-        <v>72</v>
-      </c>
+      <c r="A41" s="138"/>
       <c r="B41" s="64"/>
       <c r="C41" s="56"/>
     </row>
     <row r="42" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="145" t="s">
-        <v>64</v>
-      </c>
+      <c r="A42" s="138"/>
       <c r="B42" s="64"/>
       <c r="C42" s="56"/>
     </row>
     <row r="43" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="145" t="s">
-        <v>63</v>
-      </c>
+      <c r="A43" s="138"/>
       <c r="B43" s="64"/>
       <c r="C43" s="56"/>
     </row>
     <row r="44" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="148" t="s">
-        <v>104</v>
-      </c>
+      <c r="A44" s="141"/>
       <c r="B44" s="64"/>
       <c r="C44" s="56"/>
     </row>
     <row r="45" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="124" t="s">
-        <v>13</v>
-      </c>
+      <c r="A45" s="117"/>
       <c r="B45" s="64"/>
       <c r="C45" s="56"/>
     </row>
     <row r="46" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="158" t="s">
-        <v>47</v>
-      </c>
+      <c r="A46" s="151"/>
       <c r="B46" s="64"/>
       <c r="C46" s="56"/>
     </row>
     <row r="47" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="149" t="s">
-        <v>10</v>
-      </c>
+      <c r="A47" s="142"/>
       <c r="B47" s="28"/>
       <c r="C47" s="57"/>
     </row>
     <row r="48" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="152" t="s">
-        <v>46</v>
-      </c>
+      <c r="A48" s="145"/>
       <c r="B48" s="64"/>
       <c r="C48" s="56"/>
     </row>
     <row r="49" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="159" t="s">
-        <v>52</v>
-      </c>
+      <c r="A49" s="152"/>
       <c r="B49" s="64"/>
       <c r="C49" s="56"/>
     </row>
     <row r="50" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="149" t="s">
-        <v>41</v>
-      </c>
+      <c r="A50" s="142"/>
       <c r="B50" s="65"/>
       <c r="C50" s="56"/>
     </row>
     <row r="51" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="145" t="s">
-        <v>28</v>
-      </c>
+      <c r="A51" s="138"/>
       <c r="B51" s="64"/>
       <c r="C51" s="56"/>
     </row>
     <row r="52" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="160" t="s">
-        <v>7</v>
-      </c>
+      <c r="A52" s="153"/>
       <c r="B52" s="64"/>
       <c r="C52" s="56"/>
     </row>
     <row r="53" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="170" t="s">
-        <v>65</v>
-      </c>
+      <c r="A53" s="163"/>
       <c r="B53" s="64"/>
       <c r="C53" s="56"/>
     </row>
     <row r="54" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="149" t="s">
-        <v>97</v>
-      </c>
+      <c r="A54" s="142"/>
       <c r="B54" s="64"/>
       <c r="C54" s="56"/>
     </row>
     <row r="55" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="105" t="s">
-        <v>39</v>
-      </c>
+      <c r="A55" s="101"/>
       <c r="B55" s="64"/>
       <c r="C55" s="56"/>
     </row>
     <row r="56" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="152" t="s">
-        <v>43</v>
-      </c>
+      <c r="A56" s="145"/>
       <c r="B56" s="29"/>
       <c r="C56" s="56"/>
     </row>
     <row r="57" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="161" t="s">
-        <v>9</v>
-      </c>
+      <c r="A57" s="154"/>
       <c r="B57" s="61"/>
       <c r="C57" s="56"/>
     </row>
     <row r="58" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="162" t="s">
-        <v>44</v>
-      </c>
+      <c r="A58" s="155"/>
       <c r="B58" s="61"/>
       <c r="C58" s="56"/>
     </row>
     <row r="59" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="162" t="s">
-        <v>35</v>
-      </c>
+      <c r="A59" s="155"/>
       <c r="B59" s="61"/>
       <c r="C59" s="56"/>
     </row>
     <row r="60" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="163" t="s">
-        <v>18</v>
-      </c>
+      <c r="A60" s="156"/>
       <c r="B60" s="61"/>
       <c r="C60" s="56"/>
     </row>
     <row r="61" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="146" t="s">
-        <v>66</v>
-      </c>
+      <c r="A61" s="139"/>
       <c r="B61" s="61"/>
       <c r="C61" s="60"/>
     </row>
     <row r="62" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="152" t="s">
-        <v>99</v>
-      </c>
+      <c r="A62" s="145"/>
       <c r="B62" s="61"/>
       <c r="C62" s="56"/>
     </row>
     <row r="63" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="152" t="s">
-        <v>8</v>
-      </c>
+      <c r="A63" s="145"/>
       <c r="B63" s="61"/>
       <c r="C63" s="56"/>
     </row>
     <row r="64" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="164" t="s">
-        <v>126</v>
-      </c>
+      <c r="A64" s="157"/>
       <c r="B64" s="61"/>
       <c r="C64" s="56"/>
     </row>
     <row r="65" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="152" t="s">
-        <v>54</v>
-      </c>
+      <c r="A65" s="145"/>
       <c r="B65" s="61"/>
       <c r="C65" s="56"/>
     </row>
     <row r="66" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="164" t="s">
-        <v>11</v>
-      </c>
+      <c r="A66" s="157"/>
       <c r="B66" s="61"/>
       <c r="C66" s="56"/>
     </row>
     <row r="67" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="153" t="s">
-        <v>62</v>
-      </c>
+      <c r="A67" s="146"/>
       <c r="B67" s="61"/>
       <c r="C67" s="56"/>
     </row>
     <row r="68" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="154" t="s">
-        <v>32</v>
-      </c>
+      <c r="A68" s="147"/>
       <c r="C68" s="56"/>
     </row>
   </sheetData>
@@ -6435,6 +5851,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="c298f69c-7e32-4d69-8a4f-44b776bc75e5">
@@ -6443,15 +5868,6 @@
     <TaxCatchAll xmlns="27d18e64-52d1-4030-b5cf-9c691bb829da" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6692,20 +6108,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18B17227-D4F1-4BA2-A533-34BDC1F9C7F0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B37A3888-C326-48DF-AE4A-829BED1A658A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="c298f69c-7e32-4d69-8a4f-44b776bc75e5"/>
     <ds:schemaRef ds:uri="27d18e64-52d1-4030-b5cf-9c691bb829da"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18B17227-D4F1-4BA2-A533-34BDC1F9C7F0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
fix event logistics sheet to starrt at A88
</commit_message>
<xml_diff>
--- a/signin_templates/manager_signin.xlsx
+++ b/signin_templates/manager_signin.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brendanwoo/projects/sro_sign_in/signin_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7937D726-B971-514B-8D52-486AB1F4029A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFEB0280-1F26-8241-9813-A03C95A307DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="5" xr2:uid="{542D648B-9180-43EF-9053-182057C63D4C}"/>
+    <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{542D648B-9180-43EF-9053-182057C63D4C}"/>
   </bookViews>
   <sheets>
     <sheet name="GTWCA" sheetId="1" r:id="rId1"/>
@@ -829,7 +829,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="198">
+  <cellXfs count="196">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1329,6 +1329,60 @@
     <xf numFmtId="2" fontId="31" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="33" fillId="0" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="32" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="32" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="32" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="25" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="34" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="34" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1338,62 +1392,6 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="33" fillId="0" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="32" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="32" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="32" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="25" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="34" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="34" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -1923,6 +1921,220 @@
           <color indexed="64"/>
         </vertical>
         <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thick">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thick">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thick">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thick">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thick">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -2100,220 +2312,6 @@
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="20"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="20"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thick">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thick">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thick">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thick">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thick">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -2868,30 +2866,30 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{56F25BC1-6701-4669-AC0F-E1673995674A}" name="Table2267" displayName="Table2267" ref="A7:D29" totalsRowShown="0" headerRowDxfId="28" headerRowBorderDxfId="27" tableBorderDxfId="26" totalsRowBorderDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{56F25BC1-6701-4669-AC0F-E1673995674A}" name="Table2267" displayName="Table2267" ref="A7:D29" totalsRowShown="0" headerRowDxfId="37" headerRowBorderDxfId="36" tableBorderDxfId="35" totalsRowBorderDxfId="34">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:D29">
     <sortCondition ref="A7:A29"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="3" xr3:uid="{C0375D1B-A6A9-4878-94F1-144B367DBFAE}" name="Team " dataDxfId="24" dataCellStyle="Neutral"/>
-    <tableColumn id="1" xr3:uid="{72AB2F61-1891-C246-9F82-F99E634034BF}" name="Car #" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{731AF936-9BBC-4114-AF94-6737C2C799AD}" name="Print Name" dataDxfId="22" dataCellStyle="Neutral"/>
-    <tableColumn id="5" xr3:uid="{4AAAC599-A742-4343-8BE4-F0207EAEB236}" name="Signature" dataDxfId="21" dataCellStyle="Neutral"/>
+    <tableColumn id="3" xr3:uid="{C0375D1B-A6A9-4878-94F1-144B367DBFAE}" name="Team " dataDxfId="33" dataCellStyle="Neutral"/>
+    <tableColumn id="1" xr3:uid="{72AB2F61-1891-C246-9F82-F99E634034BF}" name="Car #" dataDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{731AF936-9BBC-4114-AF94-6737C2C799AD}" name="Print Name" dataDxfId="31" dataCellStyle="Neutral"/>
+    <tableColumn id="5" xr3:uid="{4AAAC599-A742-4343-8BE4-F0207EAEB236}" name="Signature" dataDxfId="30" dataCellStyle="Neutral"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{EEF14E4E-087A-46C7-831D-A668229E00D6}" name="Table226" displayName="Table226" ref="A7:D28" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{EEF14E4E-087A-46C7-831D-A668229E00D6}" name="Table226" displayName="Table226" ref="A7:D28" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:D28">
     <sortCondition ref="A7:A28"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="3" xr3:uid="{9FCCBAF6-EB7D-44F1-ADEC-A2DF74A549AE}" name="Team " dataDxfId="32" dataCellStyle="Neutral"/>
-    <tableColumn id="1" xr3:uid="{35983ADC-4C21-324B-8F2F-BF0F688AF0E7}" name="Car #" dataDxfId="31"/>
-    <tableColumn id="4" xr3:uid="{5972D2A1-6086-4595-9053-F6AB4ABD85A7}" name="Team Manager - Print Name" dataDxfId="30" dataCellStyle="Neutral"/>
-    <tableColumn id="7" xr3:uid="{7B3018A6-2A70-4C3E-BE5C-CCFFCABD4796}" name="Signature" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{9FCCBAF6-EB7D-44F1-ADEC-A2DF74A549AE}" name="Team " dataDxfId="24" dataCellStyle="Neutral"/>
+    <tableColumn id="1" xr3:uid="{35983ADC-4C21-324B-8F2F-BF0F688AF0E7}" name="Car #" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{5972D2A1-6086-4595-9053-F6AB4ABD85A7}" name="Team Manager - Print Name" dataDxfId="22" dataCellStyle="Neutral"/>
+    <tableColumn id="7" xr3:uid="{7B3018A6-2A70-4C3E-BE5C-CCFFCABD4796}" name="Signature" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2929,10 +2927,10 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5C8910A9-D883-CB47-ADF7-2489AEA18D68}" name="Table2" displayName="Table2" ref="A3:C68" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2">
-  <autoFilter ref="A3:C68" xr:uid="{5C8910A9-D883-CB47-ADF7-2489AEA18D68}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:C68">
-    <sortCondition ref="A3:A68"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5C8910A9-D883-CB47-ADF7-2489AEA18D68}" name="Table2" displayName="Table2" ref="A7:C72" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2">
+  <autoFilter ref="A7:C72" xr:uid="{5C8910A9-D883-CB47-ADF7-2489AEA18D68}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:C72">
+    <sortCondition ref="A7:A72"/>
   </sortState>
   <tableColumns count="3">
     <tableColumn id="2" xr3:uid="{AD000ADB-6327-CD45-BE99-F1047C0BF216}" name="Team " dataDxfId="1"/>
@@ -3245,8 +3243,8 @@
   </sheetPr>
   <dimension ref="A2:D23"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScale="60" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="60" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3259,7 +3257,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="173"/>
+      <c r="A2" s="193"/>
       <c r="B2" s="68"/>
       <c r="C2" s="169" t="s">
         <v>25</v>
@@ -3267,7 +3265,7 @@
       <c r="D2" s="169"/>
     </row>
     <row r="3" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="173"/>
+      <c r="A3" s="193"/>
       <c r="B3" s="68"/>
       <c r="C3" s="169"/>
       <c r="D3" s="169"/>
@@ -3417,18 +3415,10 @@
     <row r="2" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="68"/>
       <c r="B2" s="68"/>
-      <c r="C2" s="178" t="s">
+      <c r="C2" s="174" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="178"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C3" s="179"/>
-      <c r="D3" s="179"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C4" s="179"/>
-      <c r="D4" s="179"/>
+      <c r="D2" s="174"/>
     </row>
     <row r="7" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
@@ -3487,87 +3477,87 @@
       <c r="D14" s="7"/>
     </row>
     <row r="15" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="180"/>
+      <c r="A15" s="175"/>
       <c r="B15" s="111"/>
-      <c r="C15" s="188"/>
+      <c r="C15" s="183"/>
       <c r="D15" s="9"/>
     </row>
     <row r="16" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="181"/>
+      <c r="A16" s="176"/>
       <c r="B16" s="108"/>
-      <c r="C16" s="189"/>
+      <c r="C16" s="184"/>
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="182"/>
+      <c r="A17" s="177"/>
       <c r="B17" s="111"/>
-      <c r="C17" s="188"/>
+      <c r="C17" s="183"/>
       <c r="D17" s="98"/>
     </row>
     <row r="18" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="180"/>
+      <c r="A18" s="175"/>
       <c r="B18" s="113"/>
-      <c r="C18" s="188"/>
+      <c r="C18" s="183"/>
       <c r="D18" s="12"/>
     </row>
     <row r="19" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="183"/>
+      <c r="A19" s="178"/>
       <c r="B19" s="108"/>
-      <c r="C19" s="189"/>
+      <c r="C19" s="184"/>
       <c r="D19" s="4"/>
     </row>
     <row r="20" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="180"/>
+      <c r="A20" s="175"/>
       <c r="B20" s="114"/>
-      <c r="C20" s="188"/>
+      <c r="C20" s="183"/>
       <c r="D20" s="9"/>
     </row>
     <row r="21" spans="1:4" s="36" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="182"/>
+      <c r="A21" s="177"/>
       <c r="B21" s="108"/>
-      <c r="C21" s="188"/>
+      <c r="C21" s="183"/>
       <c r="D21" s="9"/>
     </row>
     <row r="22" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="180"/>
+      <c r="A22" s="175"/>
       <c r="B22" s="111"/>
-      <c r="C22" s="190"/>
+      <c r="C22" s="185"/>
       <c r="D22" s="12"/>
     </row>
     <row r="23" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="184"/>
+      <c r="A23" s="179"/>
       <c r="B23" s="111"/>
-      <c r="C23" s="188"/>
+      <c r="C23" s="183"/>
       <c r="D23" s="12"/>
     </row>
     <row r="24" spans="1:4" s="1" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="185"/>
+      <c r="A24" s="180"/>
       <c r="B24" s="108"/>
-      <c r="C24" s="191"/>
+      <c r="C24" s="186"/>
       <c r="D24" s="77"/>
     </row>
     <row r="25" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="186"/>
+      <c r="A25" s="181"/>
       <c r="B25" s="108"/>
-      <c r="C25" s="192"/>
+      <c r="C25" s="187"/>
       <c r="D25" s="12"/>
     </row>
     <row r="26" spans="1:4" s="36" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="181"/>
-      <c r="B26" s="194"/>
-      <c r="C26" s="193"/>
+      <c r="A26" s="176"/>
+      <c r="B26" s="189"/>
+      <c r="C26" s="188"/>
       <c r="D26" s="38"/>
     </row>
     <row r="27" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="181"/>
-      <c r="B27" s="194"/>
-      <c r="C27" s="193"/>
+      <c r="A27" s="176"/>
+      <c r="B27" s="189"/>
+      <c r="C27" s="188"/>
       <c r="D27" s="38"/>
     </row>
     <row r="28" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="187"/>
-      <c r="B28" s="195"/>
-      <c r="C28" s="189"/>
+      <c r="A28" s="182"/>
+      <c r="B28" s="190"/>
+      <c r="C28" s="184"/>
       <c r="D28" s="4"/>
     </row>
     <row r="29" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3606,26 +3596,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="173"/>
+      <c r="A2" s="193"/>
       <c r="B2" s="68"/>
     </row>
     <row r="3" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="173"/>
+      <c r="A3" s="193"/>
       <c r="B3" s="68"/>
-      <c r="C3" s="176" t="s">
+      <c r="C3" s="169" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="176"/>
+      <c r="D3" s="169"/>
     </row>
     <row r="4" spans="1:4" ht="26" x14ac:dyDescent="0.3">
-      <c r="C4" s="176"/>
-      <c r="D4" s="176"/>
+      <c r="C4" s="169"/>
+      <c r="D4" s="169"/>
     </row>
     <row r="5" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="177"/>
-      <c r="B5" s="177"/>
-      <c r="C5" s="177"/>
-      <c r="D5" s="177"/>
+      <c r="A5" s="173"/>
+      <c r="B5" s="173"/>
+      <c r="C5" s="173"/>
+      <c r="D5" s="173"/>
     </row>
     <row r="7" spans="1:4" s="1" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
@@ -3818,22 +3808,22 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:88" ht="24" x14ac:dyDescent="0.3">
-      <c r="C3" s="197" t="s">
+      <c r="C3" s="192" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="197"/>
+      <c r="D3" s="192"/>
     </row>
     <row r="4" spans="1:88" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="196"/>
-      <c r="D4" s="196"/>
+      <c r="C4" s="191"/>
+      <c r="D4" s="191"/>
     </row>
     <row r="5" spans="1:88" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C5" s="196"/>
-      <c r="D5" s="196"/>
+      <c r="C5" s="191"/>
+      <c r="D5" s="191"/>
     </row>
     <row r="6" spans="1:88" x14ac:dyDescent="0.2">
-      <c r="F6" s="173"/>
-      <c r="G6" s="173"/>
+      <c r="F6" s="193"/>
+      <c r="G6" s="193"/>
     </row>
     <row r="7" spans="1:88" s="18" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="49" t="s">
@@ -5136,12 +5126,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="174" t="s">
+      <c r="A1" s="194" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="174"/>
-      <c r="C1" s="174"/>
-      <c r="D1" s="174"/>
+      <c r="B1" s="194"/>
+      <c r="C1" s="194"/>
+      <c r="D1" s="194"/>
       <c r="E1" s="25"/>
       <c r="F1" s="25"/>
       <c r="G1" s="25"/>
@@ -5162,10 +5152,10 @@
       <c r="I2" s="25"/>
     </row>
     <row r="3" spans="1:9" ht="21" x14ac:dyDescent="0.2">
-      <c r="A3" s="175"/>
-      <c r="B3" s="175"/>
-      <c r="C3" s="175"/>
-      <c r="D3" s="175"/>
+      <c r="A3" s="195"/>
+      <c r="B3" s="195"/>
+      <c r="C3" s="195"/>
+      <c r="D3" s="195"/>
       <c r="E3" s="25"/>
       <c r="F3" s="25"/>
       <c r="G3" s="25"/>
@@ -5488,10 +5478,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C68"/>
+  <dimension ref="A1:C72"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView view="pageLayout" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5506,124 +5496,117 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="58" t="s">
+    <row r="2" spans="1:3" ht="5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="67"/>
+    </row>
+    <row r="3" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="67"/>
+    </row>
+    <row r="4" spans="1:3" ht="10" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="67"/>
+    </row>
+    <row r="5" spans="1:3" ht="1" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="67"/>
+    </row>
+    <row r="6" spans="1:3" ht="8" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="50" t="s">
+      <c r="B7" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="C7" s="59" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="140"/>
-      <c r="B4" s="61"/>
-      <c r="C4" s="56"/>
-    </row>
-    <row r="5" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="138"/>
-      <c r="B5" s="61"/>
-      <c r="C5" s="56"/>
-    </row>
-    <row r="6" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="142"/>
-      <c r="B6" s="61"/>
-      <c r="C6" s="56"/>
-    </row>
-    <row r="7" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="154"/>
-      <c r="B7" s="61"/>
-      <c r="C7" s="56"/>
-    </row>
-    <row r="8" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="148"/>
+    <row r="8" spans="1:3" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="140"/>
       <c r="B8" s="61"/>
       <c r="C8" s="56"/>
     </row>
     <row r="9" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="140"/>
+      <c r="A9" s="138"/>
       <c r="B9" s="61"/>
       <c r="C9" s="56"/>
     </row>
     <row r="10" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="141"/>
+      <c r="A10" s="142"/>
       <c r="B10" s="61"/>
       <c r="C10" s="56"/>
     </row>
     <row r="11" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="139"/>
+      <c r="A11" s="154"/>
       <c r="B11" s="61"/>
       <c r="C11" s="56"/>
     </row>
     <row r="12" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="140"/>
+      <c r="A12" s="148"/>
       <c r="B12" s="61"/>
-      <c r="C12" s="60"/>
+      <c r="C12" s="56"/>
     </row>
     <row r="13" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="52"/>
-      <c r="B13" s="64"/>
+      <c r="A13" s="140"/>
+      <c r="B13" s="61"/>
       <c r="C13" s="56"/>
     </row>
     <row r="14" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="164"/>
-      <c r="B14" s="65"/>
+      <c r="A14" s="141"/>
+      <c r="B14" s="61"/>
       <c r="C14" s="56"/>
     </row>
     <row r="15" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="142"/>
-      <c r="B15" s="64"/>
+      <c r="A15" s="139"/>
+      <c r="B15" s="61"/>
       <c r="C15" s="56"/>
     </row>
     <row r="16" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="158"/>
-      <c r="B16" s="65"/>
-      <c r="C16" s="56"/>
+      <c r="A16" s="140"/>
+      <c r="B16" s="61"/>
+      <c r="C16" s="60"/>
     </row>
     <row r="17" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="141"/>
+      <c r="A17" s="52"/>
       <c r="B17" s="64"/>
       <c r="C17" s="56"/>
     </row>
     <row r="18" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="142"/>
-      <c r="B18" s="64"/>
+      <c r="A18" s="164"/>
+      <c r="B18" s="65"/>
       <c r="C18" s="56"/>
     </row>
     <row r="19" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="144"/>
+      <c r="A19" s="142"/>
       <c r="B19" s="64"/>
       <c r="C19" s="56"/>
     </row>
     <row r="20" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="142"/>
-      <c r="B20" s="64"/>
+      <c r="A20" s="158"/>
+      <c r="B20" s="65"/>
       <c r="C20" s="56"/>
     </row>
     <row r="21" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="142"/>
+      <c r="A21" s="141"/>
       <c r="B21" s="64"/>
       <c r="C21" s="56"/>
     </row>
     <row r="22" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="141"/>
+      <c r="A22" s="142"/>
       <c r="B22" s="64"/>
       <c r="C22" s="56"/>
     </row>
     <row r="23" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="166"/>
+      <c r="A23" s="144"/>
       <c r="B23" s="64"/>
       <c r="C23" s="56"/>
     </row>
     <row r="24" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="100"/>
+      <c r="A24" s="142"/>
       <c r="B24" s="64"/>
       <c r="C24" s="56"/>
     </row>
     <row r="25" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="157"/>
+      <c r="A25" s="142"/>
       <c r="B25" s="64"/>
       <c r="C25" s="56"/>
     </row>
@@ -5633,74 +5616,74 @@
       <c r="C26" s="56"/>
     </row>
     <row r="27" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="150"/>
+      <c r="A27" s="166"/>
       <c r="B27" s="64"/>
       <c r="C27" s="56"/>
     </row>
     <row r="28" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="144"/>
+      <c r="A28" s="100"/>
       <c r="B28" s="64"/>
       <c r="C28" s="56"/>
     </row>
     <row r="29" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="140"/>
+      <c r="A29" s="157"/>
       <c r="B29" s="64"/>
       <c r="C29" s="56"/>
     </row>
     <row r="30" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="142"/>
+      <c r="A30" s="141"/>
       <c r="B30" s="64"/>
       <c r="C30" s="56"/>
     </row>
     <row r="31" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="143"/>
+      <c r="A31" s="150"/>
       <c r="B31" s="64"/>
       <c r="C31" s="56"/>
     </row>
     <row r="32" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="157"/>
+      <c r="A32" s="144"/>
       <c r="B32" s="64"/>
       <c r="C32" s="56"/>
     </row>
     <row r="33" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="141"/>
+      <c r="A33" s="140"/>
       <c r="B33" s="64"/>
       <c r="C33" s="56"/>
     </row>
     <row r="34" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="159"/>
+      <c r="A34" s="142"/>
       <c r="B34" s="64"/>
       <c r="C34" s="56"/>
     </row>
     <row r="35" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="142"/>
+      <c r="A35" s="143"/>
       <c r="B35" s="64"/>
       <c r="C35" s="56"/>
     </row>
     <row r="36" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="140"/>
-      <c r="B36" s="66"/>
+      <c r="A36" s="157"/>
+      <c r="B36" s="64"/>
       <c r="C36" s="56"/>
     </row>
     <row r="37" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="138"/>
+      <c r="A37" s="141"/>
       <c r="B37" s="64"/>
       <c r="C37" s="56"/>
     </row>
     <row r="38" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="138"/>
+      <c r="A38" s="159"/>
       <c r="B38" s="64"/>
       <c r="C38" s="56"/>
     </row>
     <row r="39" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="149"/>
+      <c r="A39" s="142"/>
       <c r="B39" s="64"/>
       <c r="C39" s="56"/>
     </row>
-    <row r="40" spans="1:3" s="162" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="63"/>
-      <c r="B40" s="160"/>
-      <c r="C40" s="161"/>
+    <row r="40" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="140"/>
+      <c r="B40" s="66"/>
+      <c r="C40" s="56"/>
     </row>
     <row r="41" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="138"/>
@@ -5713,133 +5696,153 @@
       <c r="C42" s="56"/>
     </row>
     <row r="43" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="138"/>
+      <c r="A43" s="149"/>
       <c r="B43" s="64"/>
       <c r="C43" s="56"/>
     </row>
-    <row r="44" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="141"/>
-      <c r="B44" s="64"/>
-      <c r="C44" s="56"/>
+    <row r="44" spans="1:3" s="162" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="63"/>
+      <c r="B44" s="160"/>
+      <c r="C44" s="161"/>
     </row>
     <row r="45" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="117"/>
+      <c r="A45" s="138"/>
       <c r="B45" s="64"/>
       <c r="C45" s="56"/>
     </row>
     <row r="46" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="151"/>
+      <c r="A46" s="138"/>
       <c r="B46" s="64"/>
       <c r="C46" s="56"/>
     </row>
     <row r="47" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="142"/>
-      <c r="B47" s="28"/>
-      <c r="C47" s="57"/>
+      <c r="A47" s="138"/>
+      <c r="B47" s="64"/>
+      <c r="C47" s="56"/>
     </row>
     <row r="48" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="145"/>
+      <c r="A48" s="141"/>
       <c r="B48" s="64"/>
       <c r="C48" s="56"/>
     </row>
     <row r="49" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="152"/>
+      <c r="A49" s="117"/>
       <c r="B49" s="64"/>
       <c r="C49" s="56"/>
     </row>
     <row r="50" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="142"/>
-      <c r="B50" s="65"/>
+      <c r="A50" s="151"/>
+      <c r="B50" s="64"/>
       <c r="C50" s="56"/>
     </row>
     <row r="51" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="138"/>
-      <c r="B51" s="64"/>
-      <c r="C51" s="56"/>
+      <c r="A51" s="142"/>
+      <c r="B51" s="28"/>
+      <c r="C51" s="57"/>
     </row>
     <row r="52" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="153"/>
+      <c r="A52" s="145"/>
       <c r="B52" s="64"/>
       <c r="C52" s="56"/>
     </row>
     <row r="53" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="163"/>
+      <c r="A53" s="152"/>
       <c r="B53" s="64"/>
       <c r="C53" s="56"/>
     </row>
     <row r="54" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="142"/>
-      <c r="B54" s="64"/>
+      <c r="B54" s="65"/>
       <c r="C54" s="56"/>
     </row>
     <row r="55" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="101"/>
+      <c r="A55" s="138"/>
       <c r="B55" s="64"/>
       <c r="C55" s="56"/>
     </row>
     <row r="56" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="145"/>
-      <c r="B56" s="29"/>
+      <c r="A56" s="153"/>
+      <c r="B56" s="64"/>
       <c r="C56" s="56"/>
     </row>
     <row r="57" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="154"/>
-      <c r="B57" s="61"/>
+      <c r="A57" s="163"/>
+      <c r="B57" s="64"/>
       <c r="C57" s="56"/>
     </row>
     <row r="58" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="155"/>
-      <c r="B58" s="61"/>
+      <c r="A58" s="142"/>
+      <c r="B58" s="64"/>
       <c r="C58" s="56"/>
     </row>
     <row r="59" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="155"/>
-      <c r="B59" s="61"/>
+      <c r="A59" s="101"/>
+      <c r="B59" s="64"/>
       <c r="C59" s="56"/>
     </row>
     <row r="60" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="156"/>
-      <c r="B60" s="61"/>
+      <c r="A60" s="145"/>
+      <c r="B60" s="29"/>
       <c r="C60" s="56"/>
     </row>
     <row r="61" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="139"/>
+      <c r="A61" s="154"/>
       <c r="B61" s="61"/>
-      <c r="C61" s="60"/>
+      <c r="C61" s="56"/>
     </row>
     <row r="62" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="145"/>
+      <c r="A62" s="155"/>
       <c r="B62" s="61"/>
       <c r="C62" s="56"/>
     </row>
     <row r="63" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="145"/>
+      <c r="A63" s="155"/>
       <c r="B63" s="61"/>
       <c r="C63" s="56"/>
     </row>
     <row r="64" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="157"/>
+      <c r="A64" s="156"/>
       <c r="B64" s="61"/>
       <c r="C64" s="56"/>
     </row>
     <row r="65" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="145"/>
+      <c r="A65" s="139"/>
       <c r="B65" s="61"/>
-      <c r="C65" s="56"/>
+      <c r="C65" s="60"/>
     </row>
     <row r="66" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="157"/>
+      <c r="A66" s="145"/>
       <c r="B66" s="61"/>
       <c r="C66" s="56"/>
     </row>
     <row r="67" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="146"/>
+      <c r="A67" s="145"/>
       <c r="B67" s="61"/>
       <c r="C67" s="56"/>
     </row>
     <row r="68" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="147"/>
+      <c r="A68" s="157"/>
+      <c r="B68" s="61"/>
       <c r="C68" s="56"/>
+    </row>
+    <row r="69" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="145"/>
+      <c r="B69" s="61"/>
+      <c r="C69" s="56"/>
+    </row>
+    <row r="70" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="157"/>
+      <c r="B70" s="61"/>
+      <c r="C70" s="56"/>
+    </row>
+    <row r="71" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="146"/>
+      <c r="B71" s="61"/>
+      <c r="C71" s="56"/>
+    </row>
+    <row r="72" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="147"/>
+      <c r="C72" s="56"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5851,15 +5854,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="c298f69c-7e32-4d69-8a4f-44b776bc75e5">
@@ -5868,6 +5862,15 @@
     <TaxCatchAll xmlns="27d18e64-52d1-4030-b5cf-9c691bb829da" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6108,20 +6111,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18B17227-D4F1-4BA2-A533-34BDC1F9C7F0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B37A3888-C326-48DF-AE4A-829BED1A658A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="c298f69c-7e32-4d69-8a4f-44b776bc75e5"/>
     <ds:schemaRef ds:uri="27d18e64-52d1-4030-b5cf-9c691bb829da"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18B17227-D4F1-4BA2-A533-34BDC1F9C7F0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
fix cell font sizing for event logistics
</commit_message>
<xml_diff>
--- a/signin_templates/manager_signin.xlsx
+++ b/signin_templates/manager_signin.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brendanwoo/projects/sro_sign_in/signin_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4DB8AAD-7A4F-E24C-80A5-DE6A25E2C5A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{840B4E0B-9FE9-C648-B785-D4B91601AFEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="4" xr2:uid="{542D648B-9180-43EF-9053-182057C63D4C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="5" xr2:uid="{542D648B-9180-43EF-9053-182057C63D4C}"/>
   </bookViews>
   <sheets>
     <sheet name="GTWCA" sheetId="1" r:id="rId1"/>
@@ -82,7 +82,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="46">
+  <fonts count="45" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -281,10 +281,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="16"/>
-      <name val="Calibri (Body)"/>
-    </font>
-    <font>
       <sz val="26"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -342,20 +338,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="22"/>
-      <color theme="1"/>
-      <name val="Calibri (Body)"/>
-    </font>
-    <font>
-      <sz val="22"/>
-      <name val="Calibri (Body)"/>
-    </font>
-    <font>
-      <sz val="22"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri (Body)"/>
-    </font>
-    <font>
       <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -373,6 +355,20 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="5">
@@ -718,7 +714,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="193">
+  <cellXfs count="190">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -895,9 +891,6 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="30" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -905,7 +898,7 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -978,28 +971,28 @@
     <xf numFmtId="49" fontId="22" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="32" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="33" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="34" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="33" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="32" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="31" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="31" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="32" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="32" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="33" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="34" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="32" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="33" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="31" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1014,34 +1007,34 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="36" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="2" fontId="37" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="38" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="38" fillId="0" borderId="17" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="37" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="37" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="34" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="37" fillId="0" borderId="17" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="36" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="36" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1062,80 +1055,11 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="40" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="41" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="40" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="41" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="40" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="40" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="41" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="41" fillId="0" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="42" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="41" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="42" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="41" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="43" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1145,10 +1069,10 @@
     <xf numFmtId="49" fontId="29" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="39" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="38" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="37" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="36" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1160,13 +1084,106 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="34" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="33" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="31" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="31" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="32" fillId="0" borderId="22" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="31" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="31" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="30" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="30" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="34" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="34" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="35" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="30" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="30" fillId="0" borderId="20" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="30" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="34" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="30" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="34" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="30" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="28" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="28" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1176,100 +1193,70 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="32" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="32" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="33" fillId="0" borderId="22" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="32" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="32" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="31" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="31" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="35" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="35" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="36" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="31" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="31" fillId="0" borderId="20" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="31" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="35" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="31" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="35" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="31" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="28" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="28" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="42" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="43" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="43" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="43" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="43" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="42" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="43" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="42" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="43" fillId="0" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="44" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="44" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="42" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1280,6 +1267,392 @@
     <cellStyle name="Normal 2" xfId="3" xr:uid="{561A9865-CE34-4D81-A124-2143BF703225}"/>
   </cellStyles>
   <dxfs count="48">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color auto="1"/>
+        <name val="Calibri (Body)"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thick">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thick">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thick">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thick">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thick">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="22"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="22"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thick">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thick">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thick">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thick">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thick">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1355,25 +1728,83 @@
       </border>
     </dxf>
     <dxf>
+      <border>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thick">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thick">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thick">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thick">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thick">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
+        <b/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="26"/>
-        <color theme="1"/>
+        <sz val="14"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1399,7 +1830,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="26"/>
+        <sz val="12"/>
         <color auto="1"/>
         <name val="Calibri"/>
         <family val="2"/>
@@ -1412,8 +1843,231 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thick">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thick">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thick">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thick">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thick">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1482,747 +2136,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="22"/>
-        <color auto="1"/>
-        <name val="Calibri (Body)"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thick">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thick">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thick">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thick">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thick">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="22"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="22"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thick">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thick">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thick">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thick">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thick">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thick">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thick">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thick">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thick">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thick">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="20"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="20"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thick">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thick">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thick">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thick">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thick">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border>
         <top style="thin">
           <color rgb="FF000000"/>
@@ -2342,6 +2255,80 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="26"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="26"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -2737,86 +2724,86 @@
     <sortCondition ref="A7:A19"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="3" xr3:uid="{46535ACF-119B-47E2-B654-91600EA2F824}" name="Team " dataDxfId="3" dataCellStyle="Neutral"/>
-    <tableColumn id="1" xr3:uid="{7167445C-3407-834C-B9FA-DB045AAEB2B5}" name="Car #" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{F83754C0-485E-4A3F-9902-121B9D0452B7}" name="Print Name" dataDxfId="41" dataCellStyle="Neutral"/>
-    <tableColumn id="5" xr3:uid="{B3757E69-E5A4-4C14-936E-7FBD8332261E}" name="Signature" dataDxfId="40" dataCellStyle="Neutral"/>
+    <tableColumn id="3" xr3:uid="{46535ACF-119B-47E2-B654-91600EA2F824}" name="Team " dataDxfId="41" dataCellStyle="Neutral"/>
+    <tableColumn id="1" xr3:uid="{7167445C-3407-834C-B9FA-DB045AAEB2B5}" name="Car #" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{F83754C0-485E-4A3F-9902-121B9D0452B7}" name="Print Name" dataDxfId="39" dataCellStyle="Neutral"/>
+    <tableColumn id="5" xr3:uid="{B3757E69-E5A4-4C14-936E-7FBD8332261E}" name="Signature" dataDxfId="38" dataCellStyle="Neutral"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{56F25BC1-6701-4669-AC0F-E1673995674A}" name="Table2267" displayName="Table2267" ref="A7:D38" totalsRowShown="0" headerRowDxfId="39" headerRowBorderDxfId="38" tableBorderDxfId="37" totalsRowBorderDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{56F25BC1-6701-4669-AC0F-E1673995674A}" name="Table2267" displayName="Table2267" ref="A7:D38" totalsRowShown="0" headerRowDxfId="37" headerRowBorderDxfId="36" tableBorderDxfId="35" totalsRowBorderDxfId="34">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:D29">
     <sortCondition ref="A7:A29"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="3" xr3:uid="{C0375D1B-A6A9-4878-94F1-144B367DBFAE}" name="Team " dataDxfId="5" dataCellStyle="Neutral"/>
-    <tableColumn id="1" xr3:uid="{72AB2F61-1891-C246-9F82-F99E634034BF}" name="Car #" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{731AF936-9BBC-4114-AF94-6737C2C799AD}" name="Print Name" dataDxfId="35" dataCellStyle="Neutral"/>
-    <tableColumn id="5" xr3:uid="{4AAAC599-A742-4343-8BE4-F0207EAEB236}" name="Signature" dataDxfId="34" dataCellStyle="Neutral"/>
+    <tableColumn id="3" xr3:uid="{C0375D1B-A6A9-4878-94F1-144B367DBFAE}" name="Team " dataDxfId="33" dataCellStyle="Neutral"/>
+    <tableColumn id="1" xr3:uid="{72AB2F61-1891-C246-9F82-F99E634034BF}" name="Car #" dataDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{731AF936-9BBC-4114-AF94-6737C2C799AD}" name="Print Name" dataDxfId="31" dataCellStyle="Neutral"/>
+    <tableColumn id="5" xr3:uid="{4AAAC599-A742-4343-8BE4-F0207EAEB236}" name="Signature" dataDxfId="30" dataCellStyle="Neutral"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{EEF14E4E-087A-46C7-831D-A668229E00D6}" name="Table226" displayName="Table226" ref="A7:D28" totalsRowShown="0" headerRowDxfId="33" dataDxfId="31" headerRowBorderDxfId="32" tableBorderDxfId="30" totalsRowBorderDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{EEF14E4E-087A-46C7-831D-A668229E00D6}" name="Table226" displayName="Table226" ref="A7:D28" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:D28">
     <sortCondition ref="A7:A28"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="3" xr3:uid="{9FCCBAF6-EB7D-44F1-ADEC-A2DF74A549AE}" name="Team " dataDxfId="28" dataCellStyle="Neutral"/>
-    <tableColumn id="1" xr3:uid="{35983ADC-4C21-324B-8F2F-BF0F688AF0E7}" name="Car #" dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{5972D2A1-6086-4595-9053-F6AB4ABD85A7}" name="Team Manager - Print Name" dataDxfId="26" dataCellStyle="Neutral"/>
-    <tableColumn id="7" xr3:uid="{7B3018A6-2A70-4C3E-BE5C-CCFFCABD4796}" name="Signature" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{9FCCBAF6-EB7D-44F1-ADEC-A2DF74A549AE}" name="Team " dataDxfId="24" dataCellStyle="Neutral"/>
+    <tableColumn id="1" xr3:uid="{35983ADC-4C21-324B-8F2F-BF0F688AF0E7}" name="Car #" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{5972D2A1-6086-4595-9053-F6AB4ABD85A7}" name="Team Manager - Print Name" dataDxfId="22" dataCellStyle="Neutral"/>
+    <tableColumn id="7" xr3:uid="{7B3018A6-2A70-4C3E-BE5C-CCFFCABD4796}" name="Signature" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{7C975FDB-E1BE-412D-9026-C8BCE6F82D94}" name="Table2268" displayName="Table2268" ref="A7:D26" totalsRowShown="0" headerRowDxfId="24" dataDxfId="22" headerRowBorderDxfId="23" tableBorderDxfId="21" totalsRowBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{7C975FDB-E1BE-412D-9026-C8BCE6F82D94}" name="Table2268" displayName="Table2268" ref="A7:D26" totalsRowShown="0" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:D20">
     <sortCondition ref="A8:A20"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="3" xr3:uid="{9A87D9F1-DEF9-4884-AF55-85CDAB8CC5A8}" name="Team " dataDxfId="1" dataCellStyle="Neutral"/>
-    <tableColumn id="1" xr3:uid="{A77D3C38-62D3-EB45-842F-39E925EA4278}" name="Car #" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{FB87E8C6-0099-4FD3-9EE4-DC66B1A1E154}" name="Team Manager - Print Name" dataDxfId="19" dataCellStyle="Neutral"/>
-    <tableColumn id="8" xr3:uid="{D99F6B7B-0B67-4A5D-8961-35323F63E14D}" name="Signature" dataDxfId="18" dataCellStyle="Neutral"/>
+    <tableColumn id="3" xr3:uid="{9A87D9F1-DEF9-4884-AF55-85CDAB8CC5A8}" name="Team " dataDxfId="15" dataCellStyle="Neutral"/>
+    <tableColumn id="1" xr3:uid="{A77D3C38-62D3-EB45-842F-39E925EA4278}" name="Car #" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{FB87E8C6-0099-4FD3-9EE4-DC66B1A1E154}" name="Team Manager - Print Name" dataDxfId="13" dataCellStyle="Neutral"/>
+    <tableColumn id="8" xr3:uid="{D99F6B7B-0B67-4A5D-8961-35323F63E14D}" name="Signature" dataDxfId="12" dataCellStyle="Neutral"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{34633D1F-F7E7-A54F-B80A-2DBC56A5E286}" name="Table4" displayName="Table4" ref="A5:D22" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{34633D1F-F7E7-A54F-B80A-2DBC56A5E286}" name="Table4" displayName="Table4" ref="A5:D22" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9">
   <autoFilter ref="A5:D22" xr:uid="{34633D1F-F7E7-A54F-B80A-2DBC56A5E286}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:D22">
     <sortCondition ref="A5:A22"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="2" xr3:uid="{5F92970B-06CD-C047-B9E2-6AB880B6FB5E}" name="Team " dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{54681146-35F4-D54D-9BC0-D686C4A484BC}" name="Car #" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{7B238E6B-1F96-FC45-8097-E871888A60A5}" name="Team Manager - Print Name" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{9A683F97-A1BA-904F-8CF4-974B16662D90}" name="Signature" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{5F92970B-06CD-C047-B9E2-6AB880B6FB5E}" name="Team " dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{54681146-35F4-D54D-9BC0-D686C4A484BC}" name="Car #" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{7B238E6B-1F96-FC45-8097-E871888A60A5}" name="Team Manager - Print Name" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{9A683F97-A1BA-904F-8CF4-974B16662D90}" name="Signature" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5C8910A9-D883-CB47-ADF7-2489AEA18D68}" name="Table2" displayName="Table2" ref="A7:C72" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5C8910A9-D883-CB47-ADF7-2489AEA18D68}" name="Table2" displayName="Table2" ref="A7:C72" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2">
   <autoFilter ref="A7:C72" xr:uid="{5C8910A9-D883-CB47-ADF7-2489AEA18D68}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:C72">
     <sortCondition ref="A7:A72"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="2" xr3:uid="{AD000ADB-6327-CD45-BE99-F1047C0BF216}" name="Team " dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{AD000ADB-6327-CD45-BE99-F1047C0BF216}" name="Team " dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{CDB7A7EE-F7C4-DE41-B5A3-3A45AA9CEAAC}" name="Print Name"/>
-    <tableColumn id="4" xr3:uid="{66076889-B43A-3746-B4F7-4CFF3E5423AA}" name="Signature" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{66076889-B43A-3746-B4F7-4CFF3E5423AA}" name="Signature" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3128,7 +3115,7 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="4.5" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="4.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="47.83203125" customWidth="1"/>
     <col min="2" max="2" width="31.6640625" customWidth="1"/>
@@ -3137,21 +3124,21 @@
     <col min="5" max="5" width="4.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="45" customHeight="1">
-      <c r="A2" s="158"/>
-      <c r="B2" s="67"/>
-      <c r="C2" s="150" t="s">
+    <row r="2" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="165"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="126" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="150"/>
-    </row>
-    <row r="3" spans="1:4" ht="45" customHeight="1">
-      <c r="A3" s="158"/>
-      <c r="B3" s="67"/>
-      <c r="C3" s="150"/>
-      <c r="D3" s="150"/>
-    </row>
-    <row r="7" spans="1:4" s="19" customFormat="1" ht="32.25" customHeight="1" thickBot="1">
+      <c r="D2" s="126"/>
+    </row>
+    <row r="3" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="165"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="126"/>
+      <c r="D3" s="126"/>
+    </row>
+    <row r="7" spans="1:4" s="19" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="52" t="s">
         <v>1</v>
       </c>
@@ -3165,99 +3152,99 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="19" customFormat="1" ht="46.75" customHeight="1" thickTop="1">
-      <c r="A8" s="175"/>
-      <c r="B8" s="176"/>
+    <row r="8" spans="1:4" s="19" customFormat="1" ht="46.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="148"/>
+      <c r="B8" s="149"/>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
     </row>
-    <row r="9" spans="1:4" s="19" customFormat="1" ht="46.75" customHeight="1">
-      <c r="A9" s="177"/>
-      <c r="B9" s="178"/>
+    <row r="9" spans="1:4" s="19" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="150"/>
+      <c r="B9" s="151"/>
       <c r="C9" s="21"/>
       <c r="D9" s="21"/>
     </row>
-    <row r="10" spans="1:4" s="19" customFormat="1" ht="46.75" customHeight="1">
-      <c r="A10" s="177"/>
-      <c r="B10" s="178"/>
+    <row r="10" spans="1:4" s="19" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="150"/>
+      <c r="B10" s="151"/>
       <c r="C10" s="22"/>
       <c r="D10" s="22"/>
     </row>
-    <row r="11" spans="1:4" s="19" customFormat="1" ht="46.75" customHeight="1">
-      <c r="A11" s="179"/>
-      <c r="B11" s="176"/>
+    <row r="11" spans="1:4" s="19" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="152"/>
+      <c r="B11" s="149"/>
       <c r="C11" s="21"/>
       <c r="D11" s="21"/>
     </row>
-    <row r="12" spans="1:4" s="19" customFormat="1" ht="46.75" customHeight="1">
-      <c r="A12" s="177"/>
-      <c r="B12" s="178"/>
+    <row r="12" spans="1:4" s="19" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="150"/>
+      <c r="B12" s="151"/>
       <c r="C12" s="20"/>
       <c r="D12" s="21"/>
     </row>
-    <row r="13" spans="1:4" s="19" customFormat="1" ht="46.75" customHeight="1">
-      <c r="A13" s="180"/>
-      <c r="B13" s="176"/>
+    <row r="13" spans="1:4" s="19" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="153"/>
+      <c r="B13" s="149"/>
       <c r="C13" s="21"/>
       <c r="D13" s="21"/>
     </row>
-    <row r="14" spans="1:4" s="19" customFormat="1" ht="46.75" customHeight="1">
-      <c r="A14" s="177"/>
-      <c r="B14" s="176"/>
+    <row r="14" spans="1:4" s="19" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="150"/>
+      <c r="B14" s="149"/>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
     </row>
-    <row r="15" spans="1:4" s="19" customFormat="1" ht="46.75" customHeight="1">
-      <c r="A15" s="179"/>
-      <c r="B15" s="178"/>
+    <row r="15" spans="1:4" s="19" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="152"/>
+      <c r="B15" s="151"/>
       <c r="C15" s="21"/>
       <c r="D15" s="21"/>
     </row>
-    <row r="16" spans="1:4" s="19" customFormat="1" ht="46.75" customHeight="1">
-      <c r="A16" s="177"/>
-      <c r="B16" s="178"/>
+    <row r="16" spans="1:4" s="19" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="150"/>
+      <c r="B16" s="151"/>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
     </row>
-    <row r="17" spans="1:4" s="19" customFormat="1" ht="46.75" customHeight="1">
-      <c r="A17" s="181"/>
-      <c r="B17" s="182"/>
-      <c r="C17" s="74"/>
+    <row r="17" spans="1:4" s="19" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="154"/>
+      <c r="B17" s="155"/>
+      <c r="C17" s="73"/>
       <c r="D17" s="23"/>
     </row>
-    <row r="18" spans="1:4" s="19" customFormat="1" ht="46.75" customHeight="1">
-      <c r="A18" s="183"/>
-      <c r="B18" s="178"/>
-      <c r="C18" s="73"/>
+    <row r="18" spans="1:4" s="19" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="156"/>
+      <c r="B18" s="151"/>
+      <c r="C18" s="72"/>
       <c r="D18" s="22"/>
     </row>
-    <row r="19" spans="1:4" s="19" customFormat="1" ht="46.75" customHeight="1">
-      <c r="A19" s="184"/>
-      <c r="B19" s="178"/>
+    <row r="19" spans="1:4" s="19" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="157"/>
+      <c r="B19" s="151"/>
       <c r="C19" s="20"/>
       <c r="D19" s="20"/>
     </row>
-    <row r="20" spans="1:4" ht="46.75" customHeight="1">
-      <c r="A20" s="177"/>
-      <c r="B20" s="185"/>
+    <row r="20" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="150"/>
+      <c r="B20" s="158"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
     </row>
-    <row r="21" spans="1:4" ht="46.75" customHeight="1">
-      <c r="A21" s="177"/>
-      <c r="B21" s="185"/>
+    <row r="21" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="150"/>
+      <c r="B21" s="158"/>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
     </row>
-    <row r="22" spans="1:4" ht="46.75" customHeight="1">
-      <c r="A22" s="177"/>
-      <c r="B22" s="185"/>
+    <row r="22" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="150"/>
+      <c r="B22" s="158"/>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
     </row>
-    <row r="23" spans="1:4" ht="46.75" customHeight="1">
-      <c r="A23" s="186"/>
-      <c r="B23" s="187"/>
+    <row r="23" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="159"/>
+      <c r="B23" s="160"/>
       <c r="C23" s="11"/>
       <c r="D23" s="11"/>
     </row>
@@ -3285,7 +3272,7 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="4.5" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="4.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="52.83203125" customWidth="1"/>
     <col min="2" max="2" width="29" customWidth="1"/>
@@ -3293,15 +3280,15 @@
     <col min="4" max="4" width="50.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="45" customHeight="1">
-      <c r="A2" s="67"/>
-      <c r="B2" s="67"/>
-      <c r="C2" s="152" t="s">
+    <row r="2" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="66"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="128" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="152"/>
-    </row>
-    <row r="7" spans="1:4" ht="32.25" customHeight="1" thickBot="1">
+      <c r="D2" s="128"/>
+    </row>
+    <row r="7" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
@@ -3315,189 +3302,189 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="46.75" customHeight="1" thickTop="1">
-      <c r="A8" s="162"/>
-      <c r="B8" s="91"/>
+    <row r="8" spans="1:4" ht="46.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="135"/>
+      <c r="B8" s="90"/>
       <c r="C8" s="9"/>
       <c r="D8" s="12"/>
     </row>
-    <row r="9" spans="1:4" ht="46.75" customHeight="1">
-      <c r="A9" s="163"/>
-      <c r="B9" s="92"/>
+    <row r="9" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="136"/>
+      <c r="B9" s="91"/>
       <c r="C9" s="36"/>
       <c r="D9" s="37"/>
     </row>
-    <row r="10" spans="1:4" ht="46.75" customHeight="1">
-      <c r="A10" s="164"/>
-      <c r="B10" s="112"/>
+    <row r="10" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="137"/>
+      <c r="B10" s="111"/>
       <c r="C10" s="2"/>
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:4" ht="46.75" customHeight="1">
-      <c r="A11" s="94"/>
-      <c r="B11" s="93"/>
+    <row r="11" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="93"/>
+      <c r="B11" s="92"/>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
     </row>
-    <row r="12" spans="1:4" ht="46.75" customHeight="1">
-      <c r="A12" s="94"/>
-      <c r="B12" s="94"/>
+    <row r="12" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="93"/>
+      <c r="B12" s="93"/>
       <c r="C12" s="9"/>
       <c r="D12" s="12"/>
     </row>
-    <row r="13" spans="1:4" ht="46.75" customHeight="1">
-      <c r="A13" s="165"/>
-      <c r="B13" s="95"/>
-      <c r="C13" s="85"/>
-      <c r="D13" s="87"/>
-    </row>
-    <row r="14" spans="1:4" ht="46.75" customHeight="1">
-      <c r="A14" s="90"/>
-      <c r="B14" s="96"/>
+    <row r="13" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="138"/>
+      <c r="B13" s="94"/>
+      <c r="C13" s="84"/>
+      <c r="D13" s="86"/>
+    </row>
+    <row r="14" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="89"/>
+      <c r="B14" s="95"/>
       <c r="C14" s="9"/>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4" ht="46.75" customHeight="1">
-      <c r="A15" s="166"/>
-      <c r="B15" s="96"/>
-      <c r="C15" s="153"/>
+    <row r="15" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="139"/>
+      <c r="B15" s="95"/>
+      <c r="C15" s="129"/>
       <c r="D15" s="9"/>
     </row>
-    <row r="16" spans="1:4" ht="46.75" customHeight="1">
-      <c r="A16" s="167"/>
-      <c r="B16" s="94"/>
-      <c r="C16" s="154"/>
+    <row r="16" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="140"/>
+      <c r="B16" s="93"/>
+      <c r="C16" s="130"/>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="1:4" ht="46.75" customHeight="1">
-      <c r="A17" s="168"/>
-      <c r="B17" s="96"/>
-      <c r="C17" s="153"/>
-      <c r="D17" s="86"/>
-    </row>
-    <row r="18" spans="1:4" ht="46.75" customHeight="1">
-      <c r="A18" s="166"/>
-      <c r="B18" s="97"/>
-      <c r="C18" s="153"/>
+    <row r="17" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="141"/>
+      <c r="B17" s="95"/>
+      <c r="C17" s="129"/>
+      <c r="D17" s="85"/>
+    </row>
+    <row r="18" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="139"/>
+      <c r="B18" s="96"/>
+      <c r="C18" s="129"/>
       <c r="D18" s="12"/>
     </row>
-    <row r="19" spans="1:4" ht="46.75" customHeight="1">
-      <c r="A19" s="169"/>
-      <c r="B19" s="94"/>
-      <c r="C19" s="154"/>
+    <row r="19" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="142"/>
+      <c r="B19" s="93"/>
+      <c r="C19" s="130"/>
       <c r="D19" s="4"/>
     </row>
-    <row r="20" spans="1:4" ht="46.75" customHeight="1">
-      <c r="A20" s="166"/>
-      <c r="B20" s="98"/>
-      <c r="C20" s="153"/>
+    <row r="20" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="139"/>
+      <c r="B20" s="97"/>
+      <c r="C20" s="129"/>
       <c r="D20" s="9"/>
     </row>
-    <row r="21" spans="1:4" s="35" customFormat="1" ht="46.75" customHeight="1">
-      <c r="A21" s="168"/>
-      <c r="B21" s="94"/>
-      <c r="C21" s="153"/>
+    <row r="21" spans="1:4" s="35" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="141"/>
+      <c r="B21" s="93"/>
+      <c r="C21" s="129"/>
       <c r="D21" s="9"/>
     </row>
-    <row r="22" spans="1:4" ht="46.75" customHeight="1">
-      <c r="A22" s="166"/>
-      <c r="B22" s="96"/>
+    <row r="22" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="139"/>
+      <c r="B22" s="95"/>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
     </row>
-    <row r="23" spans="1:4" ht="46.75" customHeight="1">
-      <c r="A23" s="170"/>
-      <c r="B23" s="96"/>
+    <row r="23" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="143"/>
+      <c r="B23" s="95"/>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
     </row>
-    <row r="24" spans="1:4" s="1" customFormat="1" ht="46.75" customHeight="1">
-      <c r="A24" s="161"/>
-      <c r="B24" s="94"/>
+    <row r="24" spans="1:4" s="1" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="134"/>
+      <c r="B24" s="93"/>
       <c r="C24" s="13"/>
       <c r="D24" s="13"/>
     </row>
-    <row r="25" spans="1:4" ht="46.75" customHeight="1">
-      <c r="A25" s="171"/>
-      <c r="B25" s="94"/>
+    <row r="25" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="144"/>
+      <c r="B25" s="93"/>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
     </row>
-    <row r="26" spans="1:4" s="35" customFormat="1" ht="46.75" customHeight="1">
-      <c r="A26" s="167"/>
-      <c r="B26" s="155"/>
+    <row r="26" spans="1:4" s="35" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="140"/>
+      <c r="B26" s="131"/>
       <c r="C26" s="36"/>
       <c r="D26" s="36"/>
     </row>
-    <row r="27" spans="1:4" ht="46.75" customHeight="1">
-      <c r="A27" s="167"/>
-      <c r="B27" s="155"/>
+    <row r="27" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="140"/>
+      <c r="B27" s="131"/>
       <c r="C27" s="36"/>
       <c r="D27" s="36"/>
     </row>
-    <row r="28" spans="1:4" ht="46.75" customHeight="1">
-      <c r="A28" s="172"/>
-      <c r="B28" s="155"/>
+    <row r="28" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="145"/>
+      <c r="B28" s="131"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="1:4" ht="46.75" customHeight="1">
-      <c r="A29" s="161"/>
-      <c r="B29" s="96"/>
+    <row r="29" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="134"/>
+      <c r="B29" s="95"/>
       <c r="C29" s="9"/>
       <c r="D29" s="7"/>
     </row>
-    <row r="30" spans="1:4" ht="46.75" customHeight="1">
-      <c r="A30" s="172"/>
-      <c r="B30" s="173"/>
+    <row r="30" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="145"/>
+      <c r="B30" s="146"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="1:4" ht="46.75" customHeight="1">
-      <c r="A31" s="172"/>
-      <c r="B31" s="173"/>
+    <row r="31" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="145"/>
+      <c r="B31" s="146"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="1:4" ht="46.75" customHeight="1">
-      <c r="A32" s="172"/>
-      <c r="B32" s="173"/>
+    <row r="32" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="145"/>
+      <c r="B32" s="146"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="1:4" ht="46.75" customHeight="1">
-      <c r="A33" s="172"/>
-      <c r="B33" s="173"/>
+    <row r="33" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="145"/>
+      <c r="B33" s="146"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="1:4" ht="46.75" customHeight="1">
-      <c r="A34" s="172"/>
-      <c r="B34" s="173"/>
+    <row r="34" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="145"/>
+      <c r="B34" s="146"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="1:4" ht="46.75" customHeight="1">
-      <c r="A35" s="172"/>
-      <c r="B35" s="173"/>
+    <row r="35" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="145"/>
+      <c r="B35" s="146"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="1:4" ht="46.75" customHeight="1">
-      <c r="A36" s="172"/>
-      <c r="B36" s="173"/>
+    <row r="36" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="145"/>
+      <c r="B36" s="146"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
     </row>
-    <row r="37" spans="1:4" ht="46.75" customHeight="1">
-      <c r="A37" s="172"/>
-      <c r="B37" s="173"/>
+    <row r="37" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="145"/>
+      <c r="B37" s="146"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="1:4" ht="46.75" customHeight="1">
-      <c r="A38" s="174"/>
-      <c r="B38" s="173"/>
+    <row r="38" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="147"/>
+      <c r="B38" s="146"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
     </row>
@@ -3522,7 +3509,7 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="4.5" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="4.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="48.5" customWidth="1"/>
     <col min="2" max="2" width="34" customWidth="1"/>
@@ -3530,29 +3517,29 @@
     <col min="4" max="4" width="56.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="45" customHeight="1">
-      <c r="A2" s="158"/>
-      <c r="B2" s="67"/>
-    </row>
-    <row r="3" spans="1:4" ht="45" customHeight="1">
-      <c r="A3" s="158"/>
-      <c r="B3" s="67"/>
-      <c r="C3" s="150" t="s">
+    <row r="2" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="165"/>
+      <c r="B2" s="66"/>
+    </row>
+    <row r="3" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="165"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="126" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="150"/>
-    </row>
-    <row r="4" spans="1:4" ht="26">
-      <c r="C4" s="150"/>
-      <c r="D4" s="150"/>
-    </row>
-    <row r="5" spans="1:4" ht="20.25" customHeight="1">
-      <c r="A5" s="151"/>
-      <c r="B5" s="151"/>
-      <c r="C5" s="151"/>
-      <c r="D5" s="151"/>
-    </row>
-    <row r="7" spans="1:4" s="1" customFormat="1" ht="32.25" customHeight="1" thickBot="1">
+      <c r="D3" s="126"/>
+    </row>
+    <row r="4" spans="1:4" ht="26" x14ac:dyDescent="0.3">
+      <c r="C4" s="126"/>
+      <c r="D4" s="126"/>
+    </row>
+    <row r="5" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="127"/>
+      <c r="B5" s="127"/>
+      <c r="C5" s="127"/>
+      <c r="D5" s="127"/>
+    </row>
+    <row r="7" spans="1:4" s="1" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
@@ -3566,139 +3553,139 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="5" customFormat="1" ht="36" customHeight="1" thickTop="1">
+    <row r="8" spans="1:4" s="5" customFormat="1" ht="36" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A8" s="54"/>
-      <c r="B8" s="80"/>
+      <c r="B8" s="79"/>
       <c r="C8" s="9"/>
       <c r="D8" s="13"/>
     </row>
-    <row r="9" spans="1:4" s="5" customFormat="1" ht="36" customHeight="1">
-      <c r="A9" s="72"/>
-      <c r="B9" s="80"/>
+    <row r="9" spans="1:4" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="71"/>
+      <c r="B9" s="79"/>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
     </row>
-    <row r="10" spans="1:4" s="5" customFormat="1" ht="36" customHeight="1">
+    <row r="10" spans="1:4" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="54"/>
-      <c r="B10" s="80"/>
+      <c r="B10" s="79"/>
       <c r="C10" s="9"/>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" ht="36" customHeight="1">
-      <c r="A11" s="148"/>
-      <c r="B11" s="80"/>
+    <row r="11" spans="1:4" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="124"/>
+      <c r="B11" s="79"/>
       <c r="C11" s="9"/>
       <c r="D11" s="13"/>
     </row>
-    <row r="12" spans="1:4" s="5" customFormat="1" ht="36" customHeight="1">
-      <c r="A12" s="72"/>
-      <c r="B12" s="80"/>
+    <row r="12" spans="1:4" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="71"/>
+      <c r="B12" s="79"/>
       <c r="C12" s="8"/>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4" s="5" customFormat="1" ht="36" customHeight="1">
+    <row r="13" spans="1:4" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="54"/>
       <c r="B13" s="53"/>
       <c r="C13" s="9"/>
-      <c r="D13" s="75"/>
-    </row>
-    <row r="14" spans="1:4" ht="36" customHeight="1">
-      <c r="A14" s="71"/>
-      <c r="B14" s="81"/>
+      <c r="D13" s="74"/>
+    </row>
+    <row r="14" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="70"/>
+      <c r="B14" s="80"/>
       <c r="C14" s="9"/>
-      <c r="D14" s="79"/>
-    </row>
-    <row r="15" spans="1:4" ht="36" customHeight="1">
+      <c r="D14" s="78"/>
+    </row>
+    <row r="15" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="54"/>
-      <c r="B15" s="80"/>
+      <c r="B15" s="79"/>
       <c r="C15" s="9"/>
-      <c r="D15" s="75"/>
-    </row>
-    <row r="16" spans="1:4" s="35" customFormat="1" ht="36" customHeight="1">
+      <c r="D15" s="74"/>
+    </row>
+    <row r="16" spans="1:4" s="35" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="54"/>
-      <c r="B16" s="80"/>
+      <c r="B16" s="79"/>
       <c r="C16" s="9"/>
-      <c r="D16" s="75"/>
-    </row>
-    <row r="17" spans="1:4" s="35" customFormat="1" ht="36" customHeight="1">
-      <c r="A17" s="82"/>
-      <c r="B17" s="83"/>
+      <c r="D16" s="74"/>
+    </row>
+    <row r="17" spans="1:4" s="35" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="81"/>
+      <c r="B17" s="82"/>
       <c r="C17" s="33"/>
       <c r="D17" s="13"/>
     </row>
-    <row r="18" spans="1:4" s="35" customFormat="1" ht="36" customHeight="1">
-      <c r="A18" s="82"/>
-      <c r="B18" s="83"/>
+    <row r="18" spans="1:4" s="35" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="81"/>
+      <c r="B18" s="82"/>
       <c r="C18" s="9"/>
       <c r="D18" s="13"/>
     </row>
-    <row r="19" spans="1:4" s="35" customFormat="1" ht="36" customHeight="1">
+    <row r="19" spans="1:4" s="35" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="54"/>
-      <c r="B19" s="146"/>
+      <c r="B19" s="122"/>
       <c r="C19" s="9"/>
       <c r="D19" s="13"/>
     </row>
-    <row r="20" spans="1:4" s="35" customFormat="1" ht="36" customHeight="1">
-      <c r="A20" s="71"/>
-      <c r="B20" s="81"/>
+    <row r="20" spans="1:4" s="35" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="70"/>
+      <c r="B20" s="80"/>
       <c r="C20" s="9"/>
-      <c r="D20" s="75"/>
-    </row>
-    <row r="21" spans="1:4" s="5" customFormat="1" ht="36" customHeight="1">
+      <c r="D20" s="74"/>
+    </row>
+    <row r="21" spans="1:4" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="54"/>
-      <c r="B21" s="80"/>
+      <c r="B21" s="79"/>
       <c r="C21" s="9"/>
-      <c r="D21" s="75"/>
-    </row>
-    <row r="22" spans="1:4" s="34" customFormat="1" ht="36" customHeight="1">
-      <c r="A22" s="84"/>
-      <c r="B22" s="80"/>
+      <c r="D21" s="74"/>
+    </row>
+    <row r="22" spans="1:4" s="34" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="83"/>
+      <c r="B22" s="79"/>
       <c r="C22" s="9"/>
-      <c r="D22" s="77"/>
-    </row>
-    <row r="23" spans="1:4" s="34" customFormat="1" ht="36" customHeight="1">
+      <c r="D22" s="76"/>
+    </row>
+    <row r="23" spans="1:4" s="34" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="51"/>
-      <c r="B23" s="81"/>
+      <c r="B23" s="80"/>
       <c r="C23" s="9"/>
       <c r="D23" s="13"/>
     </row>
-    <row r="24" spans="1:4" s="5" customFormat="1" ht="36" customHeight="1">
-      <c r="A24" s="84"/>
-      <c r="B24" s="80"/>
+    <row r="24" spans="1:4" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="83"/>
+      <c r="B24" s="79"/>
       <c r="C24" s="9"/>
-      <c r="D24" s="76"/>
-    </row>
-    <row r="25" spans="1:4" s="5" customFormat="1" ht="36" customHeight="1">
+      <c r="D24" s="75"/>
+    </row>
+    <row r="25" spans="1:4" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="54"/>
-      <c r="B25" s="83"/>
+      <c r="B25" s="82"/>
       <c r="C25" s="9"/>
       <c r="D25" s="13"/>
     </row>
-    <row r="26" spans="1:4" s="5" customFormat="1" ht="36" customHeight="1">
-      <c r="A26" s="82"/>
-      <c r="B26" s="83"/>
+    <row r="26" spans="1:4" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="81"/>
+      <c r="B26" s="82"/>
       <c r="C26" s="33"/>
       <c r="D26" s="46"/>
     </row>
-    <row r="27" spans="1:4" s="5" customFormat="1" ht="36" customHeight="1">
+    <row r="27" spans="1:4" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="54"/>
-      <c r="B27" s="80"/>
+      <c r="B27" s="79"/>
       <c r="C27" s="9"/>
       <c r="D27" s="13"/>
     </row>
-    <row r="28" spans="1:4" s="5" customFormat="1" ht="36" customHeight="1">
+    <row r="28" spans="1:4" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="54"/>
-      <c r="B28" s="80"/>
+      <c r="B28" s="79"/>
       <c r="C28" s="9"/>
-      <c r="D28" s="78"/>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="D28" s="77"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="14"/>
       <c r="B29" s="14"/>
       <c r="C29" s="14"/>
       <c r="D29" s="14"/>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="14"/>
       <c r="B30" s="14"/>
       <c r="C30" s="14"/>
@@ -3708,7 +3695,7 @@
   <mergeCells count="1">
     <mergeCell ref="A2:A3"/>
   </mergeCells>
-  <phoneticPr fontId="45" type="noConversion"/>
+  <phoneticPr fontId="41" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.45185185185185184" header="0.3" footer="0.3"/>
   <pageSetup scale="59" orientation="landscape" copies="2" r:id="rId1"/>
   <headerFooter>
@@ -3733,7 +3720,7 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="4.5" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="4.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="37.33203125" customWidth="1"/>
     <col min="2" max="2" width="20.5" customWidth="1"/>
@@ -3742,25 +3729,25 @@
     <col min="6" max="7" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:88" ht="24">
-      <c r="C3" s="157" t="s">
+    <row r="3" spans="1:88" ht="24" x14ac:dyDescent="0.3">
+      <c r="C3" s="133" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="157"/>
-    </row>
-    <row r="4" spans="1:88" ht="15" customHeight="1">
-      <c r="C4" s="156"/>
-      <c r="D4" s="156"/>
-    </row>
-    <row r="5" spans="1:88" ht="6" customHeight="1">
-      <c r="C5" s="156"/>
-      <c r="D5" s="156"/>
-    </row>
-    <row r="6" spans="1:88">
-      <c r="F6" s="158"/>
-      <c r="G6" s="158"/>
-    </row>
-    <row r="7" spans="1:88" s="18" customFormat="1" ht="32.25" customHeight="1" thickBot="1">
+      <c r="D3" s="133"/>
+    </row>
+    <row r="4" spans="1:88" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C4" s="132"/>
+      <c r="D4" s="132"/>
+    </row>
+    <row r="5" spans="1:88" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C5" s="132"/>
+      <c r="D5" s="132"/>
+    </row>
+    <row r="6" spans="1:88" x14ac:dyDescent="0.2">
+      <c r="F6" s="165"/>
+      <c r="G6" s="165"/>
+    </row>
+    <row r="7" spans="1:88" s="18" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="48" t="s">
         <v>1</v>
       </c>
@@ -3858,9 +3845,9 @@
       <c r="CI7" s="38"/>
       <c r="CJ7" s="39"/>
     </row>
-    <row r="8" spans="1:88" s="18" customFormat="1" ht="50.25" customHeight="1" thickTop="1">
-      <c r="A8" s="113"/>
-      <c r="B8" s="113"/>
+    <row r="8" spans="1:88" s="18" customFormat="1" ht="50.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="112"/>
+      <c r="B8" s="112"/>
       <c r="C8" s="47"/>
       <c r="D8" s="30"/>
       <c r="E8" s="38"/>
@@ -3948,9 +3935,9 @@
       <c r="CI8" s="38"/>
       <c r="CJ8" s="39"/>
     </row>
-    <row r="9" spans="1:88" s="18" customFormat="1" ht="50.25" customHeight="1">
-      <c r="A9" s="191"/>
-      <c r="B9" s="99"/>
+    <row r="9" spans="1:88" s="18" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="163"/>
+      <c r="B9" s="98"/>
       <c r="C9" s="9"/>
       <c r="D9" s="10"/>
       <c r="E9" s="38"/>
@@ -4038,9 +4025,9 @@
       <c r="CI9" s="38"/>
       <c r="CJ9" s="39"/>
     </row>
-    <row r="10" spans="1:88" s="18" customFormat="1" ht="50.25" customHeight="1">
-      <c r="A10" s="191"/>
-      <c r="B10" s="99"/>
+    <row r="10" spans="1:88" s="18" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="163"/>
+      <c r="B10" s="98"/>
       <c r="C10" s="9"/>
       <c r="D10" s="10"/>
       <c r="E10" s="38"/>
@@ -4128,11 +4115,11 @@
       <c r="CI10" s="38"/>
       <c r="CJ10" s="39"/>
     </row>
-    <row r="11" spans="1:88" s="18" customFormat="1" ht="50.25" customHeight="1">
-      <c r="A11" s="99"/>
-      <c r="B11" s="100"/>
+    <row r="11" spans="1:88" s="18" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="98"/>
+      <c r="B11" s="99"/>
       <c r="C11" s="26"/>
-      <c r="D11" s="118"/>
+      <c r="D11" s="117"/>
       <c r="E11" s="38"/>
       <c r="F11" s="38"/>
       <c r="G11" s="38"/>
@@ -4218,9 +4205,9 @@
       <c r="CI11" s="38"/>
       <c r="CJ11" s="39"/>
     </row>
-    <row r="12" spans="1:88" s="18" customFormat="1" ht="50.25" customHeight="1">
-      <c r="A12" s="114"/>
-      <c r="B12" s="102"/>
+    <row r="12" spans="1:88" s="18" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="113"/>
+      <c r="B12" s="101"/>
       <c r="C12" s="9"/>
       <c r="D12" s="10"/>
       <c r="E12" s="38"/>
@@ -4308,10 +4295,10 @@
       <c r="CI12" s="38"/>
       <c r="CJ12" s="39"/>
     </row>
-    <row r="13" spans="1:88" s="18" customFormat="1" ht="50.25" customHeight="1">
-      <c r="A13" s="89"/>
-      <c r="B13" s="102"/>
-      <c r="C13" s="117"/>
+    <row r="13" spans="1:88" s="18" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="88"/>
+      <c r="B13" s="101"/>
+      <c r="C13" s="116"/>
       <c r="D13" s="8"/>
       <c r="E13" s="38"/>
       <c r="F13" s="38"/>
@@ -4398,9 +4385,9 @@
       <c r="CI13" s="38"/>
       <c r="CJ13" s="39"/>
     </row>
-    <row r="14" spans="1:88" s="18" customFormat="1" ht="50.25" customHeight="1">
-      <c r="A14" s="89"/>
-      <c r="B14" s="99"/>
+    <row r="14" spans="1:88" s="18" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="88"/>
+      <c r="B14" s="98"/>
       <c r="C14" s="17"/>
       <c r="D14" s="45"/>
       <c r="E14" s="38"/>
@@ -4488,9 +4475,9 @@
       <c r="CI14" s="38"/>
       <c r="CJ14" s="39"/>
     </row>
-    <row r="15" spans="1:88" s="18" customFormat="1" ht="50.25" customHeight="1">
-      <c r="A15" s="89"/>
-      <c r="B15" s="99"/>
+    <row r="15" spans="1:88" s="18" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="88"/>
+      <c r="B15" s="98"/>
       <c r="C15" s="17"/>
       <c r="D15" s="16"/>
       <c r="E15" s="38"/>
@@ -4578,9 +4565,9 @@
       <c r="CI15" s="38"/>
       <c r="CJ15" s="39"/>
     </row>
-    <row r="16" spans="1:88" s="18" customFormat="1" ht="50.25" customHeight="1">
-      <c r="A16" s="191"/>
-      <c r="B16" s="145"/>
+    <row r="16" spans="1:88" s="18" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="163"/>
+      <c r="B16" s="121"/>
       <c r="C16" s="9"/>
       <c r="D16" s="44"/>
       <c r="E16" s="38"/>
@@ -4668,9 +4655,9 @@
       <c r="CI16" s="38"/>
       <c r="CJ16" s="39"/>
     </row>
-    <row r="17" spans="1:88" s="18" customFormat="1" ht="50.25" customHeight="1">
-      <c r="A17" s="89"/>
-      <c r="B17" s="116"/>
+    <row r="17" spans="1:88" s="18" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="88"/>
+      <c r="B17" s="115"/>
       <c r="C17" s="17"/>
       <c r="D17" s="10"/>
       <c r="E17" s="38"/>
@@ -4758,10 +4745,10 @@
       <c r="CI17" s="38"/>
       <c r="CJ17" s="39"/>
     </row>
-    <row r="18" spans="1:88" s="42" customFormat="1" ht="50.25" customHeight="1">
-      <c r="A18" s="88"/>
-      <c r="B18" s="115"/>
-      <c r="C18" s="117"/>
+    <row r="18" spans="1:88" s="42" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="87"/>
+      <c r="B18" s="114"/>
+      <c r="C18" s="116"/>
       <c r="D18" s="10"/>
       <c r="E18" s="41"/>
       <c r="F18" s="41"/>
@@ -4848,9 +4835,9 @@
       <c r="CI18" s="41"/>
       <c r="CJ18" s="43"/>
     </row>
-    <row r="19" spans="1:88" s="42" customFormat="1" ht="50.25" customHeight="1">
-      <c r="A19" s="89"/>
-      <c r="B19" s="101"/>
+    <row r="19" spans="1:88" s="42" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="88"/>
+      <c r="B19" s="100"/>
       <c r="C19" s="10"/>
       <c r="D19" s="8"/>
       <c r="E19" s="41"/>
@@ -4938,9 +4925,9 @@
       <c r="CI19" s="41"/>
       <c r="CJ19" s="43"/>
     </row>
-    <row r="20" spans="1:88" s="18" customFormat="1" ht="50.25" customHeight="1">
-      <c r="A20" s="89"/>
-      <c r="B20" s="99"/>
+    <row r="20" spans="1:88" s="18" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="88"/>
+      <c r="B20" s="98"/>
       <c r="C20" s="15"/>
       <c r="D20" s="16"/>
       <c r="E20" s="38"/>
@@ -5028,41 +5015,41 @@
       <c r="CI20" s="38"/>
       <c r="CJ20" s="39"/>
     </row>
-    <row r="21" spans="1:88" ht="50.25" customHeight="1">
-      <c r="A21" s="191"/>
-      <c r="B21" s="188"/>
+    <row r="21" spans="1:88" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="163"/>
+      <c r="B21" s="98"/>
       <c r="C21" s="9"/>
       <c r="D21" s="10"/>
     </row>
-    <row r="22" spans="1:88" ht="50.25" customHeight="1">
-      <c r="A22" s="191"/>
-      <c r="B22" s="188"/>
+    <row r="22" spans="1:88" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="163"/>
+      <c r="B22" s="98"/>
       <c r="C22" s="9"/>
       <c r="D22" s="10"/>
     </row>
-    <row r="23" spans="1:88" ht="50.25" customHeight="1">
-      <c r="A23" s="191"/>
-      <c r="B23" s="188"/>
+    <row r="23" spans="1:88" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="163"/>
+      <c r="B23" s="98"/>
       <c r="C23" s="9"/>
       <c r="D23" s="10"/>
     </row>
-    <row r="24" spans="1:88" ht="50.25" customHeight="1">
-      <c r="A24" s="191"/>
-      <c r="B24" s="188"/>
+    <row r="24" spans="1:88" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="163"/>
+      <c r="B24" s="98"/>
       <c r="C24" s="9"/>
       <c r="D24" s="10"/>
     </row>
-    <row r="25" spans="1:88" ht="50.25" customHeight="1">
-      <c r="A25" s="191"/>
-      <c r="B25" s="188"/>
+    <row r="25" spans="1:88" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="163"/>
+      <c r="B25" s="98"/>
       <c r="C25" s="9"/>
       <c r="D25" s="10"/>
     </row>
-    <row r="26" spans="1:88" ht="50.25" customHeight="1">
-      <c r="A26" s="192"/>
-      <c r="B26" s="189"/>
+    <row r="26" spans="1:88" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="164"/>
+      <c r="B26" s="161"/>
       <c r="C26" s="11"/>
-      <c r="D26" s="190"/>
+      <c r="D26" s="162"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5084,11 +5071,11 @@
   </sheetPr>
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="50" zoomScaleNormal="80" zoomScalePageLayoutView="50" workbookViewId="0">
+    <sheetView view="pageLayout" zoomScale="50" zoomScaleNormal="80" zoomScalePageLayoutView="50" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="47.6640625" style="31" customWidth="1"/>
     <col min="3" max="3" width="62.83203125" style="29" customWidth="1"/>
@@ -5096,20 +5083,20 @@
     <col min="5" max="16384" width="9.1640625" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="63" customHeight="1">
-      <c r="A1" s="159" t="s">
+    <row r="1" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="166" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="159"/>
-      <c r="C1" s="159"/>
-      <c r="D1" s="159"/>
+      <c r="B1" s="166"/>
+      <c r="C1" s="166"/>
+      <c r="D1" s="166"/>
       <c r="E1" s="25"/>
       <c r="F1" s="25"/>
       <c r="G1" s="25"/>
       <c r="H1" s="25"/>
       <c r="I1" s="25"/>
     </row>
-    <row r="2" spans="1:9" ht="15.75" hidden="1" customHeight="1">
+    <row r="2" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="30"/>
       <c r="B2" s="30"/>
       <c r="C2" s="32" t="s">
@@ -5122,18 +5109,18 @@
       <c r="H2" s="25"/>
       <c r="I2" s="25"/>
     </row>
-    <row r="3" spans="1:9" ht="21">
-      <c r="A3" s="160"/>
-      <c r="B3" s="160"/>
-      <c r="C3" s="160"/>
-      <c r="D3" s="160"/>
+    <row r="3" spans="1:9" ht="21" x14ac:dyDescent="0.2">
+      <c r="A3" s="167"/>
+      <c r="B3" s="167"/>
+      <c r="C3" s="167"/>
+      <c r="D3" s="167"/>
       <c r="E3" s="25"/>
       <c r="F3" s="25"/>
       <c r="G3" s="25"/>
       <c r="H3" s="25"/>
       <c r="I3" s="25"/>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1">
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="30"/>
       <c r="B4" s="30"/>
       <c r="C4" s="25"/>
@@ -5144,11 +5131,11 @@
       <c r="H4" s="25"/>
       <c r="I4" s="25"/>
     </row>
-    <row r="5" spans="1:9" ht="33" customHeight="1" thickBot="1">
+    <row r="5" spans="1:9" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="68" t="s">
+      <c r="B5" s="67" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="49" t="s">
@@ -5163,9 +5150,9 @@
       <c r="H5" s="25"/>
       <c r="I5" s="25"/>
     </row>
-    <row r="6" spans="1:9" ht="57.5" customHeight="1" thickTop="1">
-      <c r="A6" s="103"/>
-      <c r="B6" s="109"/>
+    <row r="6" spans="1:9" ht="57.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="102"/>
+      <c r="B6" s="108"/>
       <c r="C6" s="28"/>
       <c r="D6" s="55"/>
       <c r="E6" s="25"/>
@@ -5174,9 +5161,9 @@
       <c r="H6" s="25"/>
       <c r="I6" s="25"/>
     </row>
-    <row r="7" spans="1:9" ht="57.5" customHeight="1">
-      <c r="A7" s="105"/>
-      <c r="B7" s="106"/>
+    <row r="7" spans="1:9" ht="57.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="104"/>
+      <c r="B7" s="105"/>
       <c r="C7" s="24"/>
       <c r="D7" s="25"/>
       <c r="E7" s="25"/>
@@ -5185,9 +5172,9 @@
       <c r="H7" s="25"/>
       <c r="I7" s="25"/>
     </row>
-    <row r="8" spans="1:9" ht="57.5" customHeight="1">
-      <c r="A8" s="105"/>
-      <c r="B8" s="107"/>
+    <row r="8" spans="1:9" ht="57.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="104"/>
+      <c r="B8" s="106"/>
       <c r="C8" s="24"/>
       <c r="D8" s="61"/>
       <c r="E8" s="25"/>
@@ -5196,9 +5183,9 @@
       <c r="H8" s="25"/>
       <c r="I8" s="25"/>
     </row>
-    <row r="9" spans="1:9" ht="57.5" customHeight="1">
-      <c r="A9" s="105"/>
-      <c r="B9" s="108"/>
+    <row r="9" spans="1:9" ht="57.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="104"/>
+      <c r="B9" s="107"/>
       <c r="C9" s="24"/>
       <c r="D9" s="55"/>
       <c r="E9" s="25"/>
@@ -5207,9 +5194,9 @@
       <c r="H9" s="25"/>
       <c r="I9" s="25"/>
     </row>
-    <row r="10" spans="1:9" ht="57.5" customHeight="1">
-      <c r="A10" s="103"/>
-      <c r="B10" s="104"/>
+    <row r="10" spans="1:9" ht="57.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="102"/>
+      <c r="B10" s="103"/>
       <c r="C10" s="28"/>
       <c r="D10" s="55"/>
       <c r="E10" s="25"/>
@@ -5218,9 +5205,9 @@
       <c r="H10" s="25"/>
       <c r="I10" s="25"/>
     </row>
-    <row r="11" spans="1:9" ht="57.5" customHeight="1">
-      <c r="A11" s="103"/>
-      <c r="B11" s="104"/>
+    <row r="11" spans="1:9" ht="57.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="102"/>
+      <c r="B11" s="103"/>
       <c r="C11" s="28"/>
       <c r="D11" s="55"/>
       <c r="E11" s="25"/>
@@ -5229,9 +5216,9 @@
       <c r="H11" s="25"/>
       <c r="I11" s="25"/>
     </row>
-    <row r="12" spans="1:9" ht="57.5" customHeight="1">
-      <c r="A12" s="103"/>
-      <c r="B12" s="104"/>
+    <row r="12" spans="1:9" ht="57.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="102"/>
+      <c r="B12" s="103"/>
       <c r="C12" s="28"/>
       <c r="D12" s="55"/>
       <c r="E12" s="25"/>
@@ -5240,9 +5227,9 @@
       <c r="H12" s="25"/>
       <c r="I12" s="25"/>
     </row>
-    <row r="13" spans="1:9" ht="57.5" customHeight="1">
-      <c r="A13" s="103"/>
-      <c r="B13" s="104"/>
+    <row r="13" spans="1:9" ht="57.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="102"/>
+      <c r="B13" s="103"/>
       <c r="C13" s="28"/>
       <c r="D13" s="55"/>
       <c r="E13" s="25"/>
@@ -5251,9 +5238,9 @@
       <c r="H13" s="25"/>
       <c r="I13" s="25"/>
     </row>
-    <row r="14" spans="1:9" ht="57.5" customHeight="1">
-      <c r="A14" s="103"/>
-      <c r="B14" s="109"/>
+    <row r="14" spans="1:9" ht="57.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="102"/>
+      <c r="B14" s="108"/>
       <c r="C14" s="28"/>
       <c r="D14" s="55"/>
       <c r="E14" s="25"/>
@@ -5262,9 +5249,9 @@
       <c r="H14" s="25"/>
       <c r="I14" s="25"/>
     </row>
-    <row r="15" spans="1:9" ht="57.5" customHeight="1">
-      <c r="A15" s="105"/>
-      <c r="B15" s="106"/>
+    <row r="15" spans="1:9" ht="57.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="104"/>
+      <c r="B15" s="105"/>
       <c r="C15" s="24"/>
       <c r="D15" s="56"/>
       <c r="E15" s="25"/>
@@ -5273,9 +5260,9 @@
       <c r="H15" s="25"/>
       <c r="I15" s="25"/>
     </row>
-    <row r="16" spans="1:9" ht="57.5" customHeight="1">
+    <row r="16" spans="1:9" ht="57.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="50"/>
-      <c r="B16" s="104"/>
+      <c r="B16" s="103"/>
       <c r="C16" s="28"/>
       <c r="D16" s="55"/>
       <c r="E16" s="25"/>
@@ -5284,9 +5271,9 @@
       <c r="H16" s="25"/>
       <c r="I16" s="25"/>
     </row>
-    <row r="17" spans="1:9" ht="57.5" customHeight="1">
-      <c r="A17" s="88"/>
-      <c r="B17" s="149"/>
+    <row r="17" spans="1:9" ht="57.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="87"/>
+      <c r="B17" s="125"/>
       <c r="C17" s="24"/>
       <c r="D17" s="55"/>
       <c r="E17" s="25"/>
@@ -5295,9 +5282,9 @@
       <c r="H17" s="25"/>
       <c r="I17" s="25"/>
     </row>
-    <row r="18" spans="1:9" ht="57.5" customHeight="1">
-      <c r="A18" s="103"/>
-      <c r="B18" s="104"/>
+    <row r="18" spans="1:9" ht="57.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="102"/>
+      <c r="B18" s="103"/>
       <c r="C18" s="28"/>
       <c r="D18" s="55"/>
       <c r="E18" s="25"/>
@@ -5306,9 +5293,9 @@
       <c r="H18" s="25"/>
       <c r="I18" s="25"/>
     </row>
-    <row r="19" spans="1:9" ht="57.5" customHeight="1">
-      <c r="A19" s="103"/>
-      <c r="B19" s="104"/>
+    <row r="19" spans="1:9" ht="57.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="102"/>
+      <c r="B19" s="103"/>
       <c r="C19" s="24"/>
       <c r="D19" s="55"/>
       <c r="E19" s="25"/>
@@ -5317,9 +5304,9 @@
       <c r="H19" s="25"/>
       <c r="I19" s="25"/>
     </row>
-    <row r="20" spans="1:9" ht="57.5" customHeight="1">
-      <c r="A20" s="103"/>
-      <c r="B20" s="104"/>
+    <row r="20" spans="1:9" ht="57.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="102"/>
+      <c r="B20" s="103"/>
       <c r="C20" s="28"/>
       <c r="D20" s="55"/>
       <c r="E20" s="25"/>
@@ -5328,10 +5315,10 @@
       <c r="H20" s="25"/>
       <c r="I20" s="25"/>
     </row>
-    <row r="21" spans="1:9" ht="57.5" customHeight="1">
-      <c r="A21" s="103"/>
-      <c r="B21" s="104"/>
-      <c r="C21" s="69"/>
+    <row r="21" spans="1:9" ht="57.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="102"/>
+      <c r="B21" s="103"/>
+      <c r="C21" s="68"/>
       <c r="D21" s="55"/>
       <c r="E21" s="25"/>
       <c r="F21" s="25"/>
@@ -5339,10 +5326,10 @@
       <c r="H21" s="25"/>
       <c r="I21" s="25"/>
     </row>
-    <row r="22" spans="1:9" ht="57.5" customHeight="1">
-      <c r="A22" s="110"/>
-      <c r="B22" s="111"/>
-      <c r="C22" s="70"/>
+    <row r="22" spans="1:9" ht="57.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="109"/>
+      <c r="B22" s="110"/>
+      <c r="C22" s="69"/>
       <c r="D22" s="59"/>
       <c r="E22" s="25"/>
       <c r="F22" s="25"/>
@@ -5350,13 +5337,13 @@
       <c r="H22" s="25"/>
       <c r="I22" s="25"/>
     </row>
-    <row r="23" spans="1:9" ht="27" customHeight="1">
+    <row r="23" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="30"/>
       <c r="B23" s="30"/>
       <c r="C23" s="25"/>
       <c r="D23" s="25"/>
     </row>
-    <row r="24" spans="1:9" ht="27" customHeight="1">
+    <row r="24" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="30"/>
       <c r="B24" s="30"/>
       <c r="C24" s="25"/>
@@ -5383,36 +5370,36 @@
   </sheetPr>
   <dimension ref="A1:C72"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="38.83203125" customWidth="1"/>
     <col min="2" max="2" width="47.1640625" customWidth="1"/>
     <col min="3" max="3" width="42" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="92" customHeight="1">
-      <c r="B1" s="66" t="s">
+    <row r="1" spans="1:3" ht="92" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B1" s="65" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="5" customHeight="1">
-      <c r="B2" s="66"/>
-    </row>
-    <row r="3" spans="1:3" ht="14" customHeight="1">
-      <c r="B3" s="66"/>
-    </row>
-    <row r="4" spans="1:3" ht="10" hidden="1" customHeight="1">
-      <c r="B4" s="66"/>
-    </row>
-    <row r="5" spans="1:3" ht="1" hidden="1" customHeight="1">
-      <c r="B5" s="66"/>
-    </row>
-    <row r="6" spans="1:3" ht="8" customHeight="1"/>
-    <row r="7" spans="1:3" ht="21" thickBot="1">
+    <row r="2" spans="1:3" ht="5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="65"/>
+    </row>
+    <row r="3" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="65"/>
+    </row>
+    <row r="4" spans="1:3" ht="10" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="65"/>
+    </row>
+    <row r="5" spans="1:3" ht="1" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="65"/>
+    </row>
+    <row r="6" spans="1:3" ht="8" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="57" t="s">
         <v>1</v>
       </c>
@@ -5423,328 +5410,328 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="40" customHeight="1" thickTop="1">
-      <c r="A8" s="121"/>
+    <row r="8" spans="1:3" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="168"/>
       <c r="B8" s="60"/>
       <c r="C8" s="55"/>
     </row>
-    <row r="9" spans="1:3" ht="40" customHeight="1">
-      <c r="A9" s="119"/>
+    <row r="9" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="169"/>
       <c r="B9" s="60"/>
       <c r="C9" s="55"/>
     </row>
-    <row r="10" spans="1:3" ht="40" customHeight="1">
-      <c r="A10" s="123"/>
+    <row r="10" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="170"/>
       <c r="B10" s="60"/>
       <c r="C10" s="55"/>
     </row>
-    <row r="11" spans="1:3" ht="40" customHeight="1">
-      <c r="A11" s="135"/>
+    <row r="11" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="171"/>
       <c r="B11" s="60"/>
       <c r="C11" s="55"/>
     </row>
-    <row r="12" spans="1:3" ht="40" customHeight="1">
-      <c r="A12" s="129"/>
+    <row r="12" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="172"/>
       <c r="B12" s="60"/>
       <c r="C12" s="55"/>
     </row>
-    <row r="13" spans="1:3" ht="40" customHeight="1">
-      <c r="A13" s="121"/>
+    <row r="13" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="168"/>
       <c r="B13" s="60"/>
       <c r="C13" s="55"/>
     </row>
-    <row r="14" spans="1:3" ht="40" customHeight="1">
-      <c r="A14" s="122"/>
+    <row r="14" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="173"/>
       <c r="B14" s="60"/>
       <c r="C14" s="55"/>
     </row>
-    <row r="15" spans="1:3" ht="40" customHeight="1">
-      <c r="A15" s="120"/>
+    <row r="15" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="174"/>
       <c r="B15" s="60"/>
       <c r="C15" s="55"/>
     </row>
-    <row r="16" spans="1:3" ht="40" customHeight="1">
-      <c r="A16" s="121"/>
+    <row r="16" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="168"/>
       <c r="B16" s="60"/>
       <c r="C16" s="59"/>
     </row>
-    <row r="17" spans="1:3" ht="40" customHeight="1">
-      <c r="A17" s="51"/>
-      <c r="B17" s="63"/>
+    <row r="17" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="175"/>
+      <c r="B17" s="62"/>
       <c r="C17" s="55"/>
     </row>
-    <row r="18" spans="1:3" ht="40" customHeight="1">
-      <c r="A18" s="145"/>
-      <c r="B18" s="64"/>
+    <row r="18" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="121"/>
+      <c r="B18" s="63"/>
       <c r="C18" s="55"/>
     </row>
-    <row r="19" spans="1:3" ht="40" customHeight="1">
-      <c r="A19" s="123"/>
-      <c r="B19" s="63"/>
+    <row r="19" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="170"/>
+      <c r="B19" s="62"/>
       <c r="C19" s="55"/>
     </row>
-    <row r="20" spans="1:3" ht="40" customHeight="1">
-      <c r="A20" s="139"/>
-      <c r="B20" s="64"/>
+    <row r="20" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="87"/>
+      <c r="B20" s="63"/>
       <c r="C20" s="55"/>
     </row>
-    <row r="21" spans="1:3" ht="40" customHeight="1">
-      <c r="A21" s="122"/>
-      <c r="B21" s="63"/>
+    <row r="21" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="173"/>
+      <c r="B21" s="62"/>
       <c r="C21" s="55"/>
     </row>
-    <row r="22" spans="1:3" ht="40" customHeight="1">
-      <c r="A22" s="123"/>
-      <c r="B22" s="63"/>
+    <row r="22" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="170"/>
+      <c r="B22" s="62"/>
       <c r="C22" s="55"/>
     </row>
-    <row r="23" spans="1:3" ht="40" customHeight="1">
-      <c r="A23" s="125"/>
-      <c r="B23" s="63"/>
+    <row r="23" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="176"/>
+      <c r="B23" s="62"/>
       <c r="C23" s="55"/>
     </row>
-    <row r="24" spans="1:3" ht="40" customHeight="1">
-      <c r="A24" s="123"/>
-      <c r="B24" s="63"/>
+    <row r="24" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="170"/>
+      <c r="B24" s="62"/>
       <c r="C24" s="55"/>
     </row>
-    <row r="25" spans="1:3" ht="40" customHeight="1">
-      <c r="A25" s="123"/>
-      <c r="B25" s="63"/>
+    <row r="25" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="170"/>
+      <c r="B25" s="62"/>
       <c r="C25" s="55"/>
     </row>
-    <row r="26" spans="1:3" ht="40" customHeight="1">
-      <c r="A26" s="122"/>
-      <c r="B26" s="63"/>
+    <row r="26" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="173"/>
+      <c r="B26" s="62"/>
       <c r="C26" s="55"/>
     </row>
-    <row r="27" spans="1:3" ht="40" customHeight="1">
-      <c r="A27" s="147"/>
-      <c r="B27" s="63"/>
+    <row r="27" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="123"/>
+      <c r="B27" s="62"/>
       <c r="C27" s="55"/>
     </row>
-    <row r="28" spans="1:3" ht="40" customHeight="1">
-      <c r="A28" s="88"/>
-      <c r="B28" s="63"/>
+    <row r="28" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="87"/>
+      <c r="B28" s="62"/>
       <c r="C28" s="55"/>
     </row>
-    <row r="29" spans="1:3" ht="40" customHeight="1">
-      <c r="A29" s="138"/>
-      <c r="B29" s="63"/>
+    <row r="29" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="177"/>
+      <c r="B29" s="62"/>
       <c r="C29" s="55"/>
     </row>
-    <row r="30" spans="1:3" ht="40" customHeight="1">
-      <c r="A30" s="122"/>
-      <c r="B30" s="63"/>
+    <row r="30" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="173"/>
+      <c r="B30" s="62"/>
       <c r="C30" s="55"/>
     </row>
-    <row r="31" spans="1:3" ht="40" customHeight="1">
-      <c r="A31" s="131"/>
-      <c r="B31" s="63"/>
+    <row r="31" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="178"/>
+      <c r="B31" s="62"/>
       <c r="C31" s="55"/>
     </row>
-    <row r="32" spans="1:3" ht="40" customHeight="1">
-      <c r="A32" s="125"/>
-      <c r="B32" s="63"/>
+    <row r="32" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="176"/>
+      <c r="B32" s="62"/>
       <c r="C32" s="55"/>
     </row>
-    <row r="33" spans="1:3" ht="40" customHeight="1">
-      <c r="A33" s="121"/>
-      <c r="B33" s="63"/>
+    <row r="33" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="168"/>
+      <c r="B33" s="62"/>
       <c r="C33" s="55"/>
     </row>
-    <row r="34" spans="1:3" ht="40" customHeight="1">
-      <c r="A34" s="123"/>
-      <c r="B34" s="63"/>
+    <row r="34" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="170"/>
+      <c r="B34" s="62"/>
       <c r="C34" s="55"/>
     </row>
-    <row r="35" spans="1:3" ht="40" customHeight="1">
-      <c r="A35" s="124"/>
-      <c r="B35" s="63"/>
+    <row r="35" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="179"/>
+      <c r="B35" s="62"/>
       <c r="C35" s="55"/>
     </row>
-    <row r="36" spans="1:3" ht="40" customHeight="1">
-      <c r="A36" s="138"/>
-      <c r="B36" s="63"/>
+    <row r="36" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="177"/>
+      <c r="B36" s="62"/>
       <c r="C36" s="55"/>
     </row>
-    <row r="37" spans="1:3" ht="40" customHeight="1">
-      <c r="A37" s="122"/>
-      <c r="B37" s="63"/>
+    <row r="37" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="173"/>
+      <c r="B37" s="62"/>
       <c r="C37" s="55"/>
     </row>
-    <row r="38" spans="1:3" ht="40" customHeight="1">
-      <c r="A38" s="140"/>
-      <c r="B38" s="63"/>
+    <row r="38" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="180"/>
+      <c r="B38" s="62"/>
       <c r="C38" s="55"/>
     </row>
-    <row r="39" spans="1:3" ht="40" customHeight="1">
-      <c r="A39" s="123"/>
-      <c r="B39" s="63"/>
+    <row r="39" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="170"/>
+      <c r="B39" s="62"/>
       <c r="C39" s="55"/>
     </row>
-    <row r="40" spans="1:3" ht="40" customHeight="1">
-      <c r="A40" s="121"/>
-      <c r="B40" s="65"/>
+    <row r="40" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="168"/>
+      <c r="B40" s="64"/>
       <c r="C40" s="55"/>
     </row>
-    <row r="41" spans="1:3" ht="40" customHeight="1">
-      <c r="A41" s="119"/>
-      <c r="B41" s="63"/>
+    <row r="41" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="169"/>
+      <c r="B41" s="62"/>
       <c r="C41" s="55"/>
     </row>
-    <row r="42" spans="1:3" ht="40" customHeight="1">
-      <c r="A42" s="119"/>
-      <c r="B42" s="63"/>
+    <row r="42" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="169"/>
+      <c r="B42" s="62"/>
       <c r="C42" s="55"/>
     </row>
-    <row r="43" spans="1:3" ht="40" customHeight="1">
-      <c r="A43" s="130"/>
-      <c r="B43" s="63"/>
+    <row r="43" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="181"/>
+      <c r="B43" s="62"/>
       <c r="C43" s="55"/>
     </row>
-    <row r="44" spans="1:3" s="143" customFormat="1" ht="40" customHeight="1">
-      <c r="A44" s="62"/>
-      <c r="B44" s="141"/>
-      <c r="C44" s="142"/>
-    </row>
-    <row r="45" spans="1:3" ht="40" customHeight="1">
-      <c r="A45" s="119"/>
-      <c r="B45" s="63"/>
+    <row r="44" spans="1:3" s="120" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="176"/>
+      <c r="B44" s="118"/>
+      <c r="C44" s="119"/>
+    </row>
+    <row r="45" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="169"/>
+      <c r="B45" s="62"/>
       <c r="C45" s="55"/>
     </row>
-    <row r="46" spans="1:3" ht="40" customHeight="1">
-      <c r="A46" s="119"/>
-      <c r="B46" s="63"/>
+    <row r="46" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="169"/>
+      <c r="B46" s="62"/>
       <c r="C46" s="55"/>
     </row>
-    <row r="47" spans="1:3" ht="40" customHeight="1">
-      <c r="A47" s="119"/>
-      <c r="B47" s="63"/>
+    <row r="47" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="169"/>
+      <c r="B47" s="62"/>
       <c r="C47" s="55"/>
     </row>
-    <row r="48" spans="1:3" ht="40" customHeight="1">
-      <c r="A48" s="122"/>
-      <c r="B48" s="63"/>
+    <row r="48" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="173"/>
+      <c r="B48" s="62"/>
       <c r="C48" s="55"/>
     </row>
-    <row r="49" spans="1:3" ht="40" customHeight="1">
-      <c r="A49" s="99"/>
-      <c r="B49" s="63"/>
+    <row r="49" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="98"/>
+      <c r="B49" s="62"/>
       <c r="C49" s="55"/>
     </row>
-    <row r="50" spans="1:3" ht="40" customHeight="1">
-      <c r="A50" s="132"/>
-      <c r="B50" s="63"/>
+    <row r="50" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="182"/>
+      <c r="B50" s="62"/>
       <c r="C50" s="55"/>
     </row>
-    <row r="51" spans="1:3" ht="40" customHeight="1">
-      <c r="A51" s="123"/>
+    <row r="51" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="170"/>
       <c r="B51" s="27"/>
       <c r="C51" s="56"/>
     </row>
-    <row r="52" spans="1:3" ht="40" customHeight="1">
-      <c r="A52" s="126"/>
-      <c r="B52" s="63"/>
+    <row r="52" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="183"/>
+      <c r="B52" s="62"/>
       <c r="C52" s="55"/>
     </row>
-    <row r="53" spans="1:3" ht="40" customHeight="1">
-      <c r="A53" s="133"/>
-      <c r="B53" s="63"/>
+    <row r="53" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="184"/>
+      <c r="B53" s="62"/>
       <c r="C53" s="55"/>
     </row>
-    <row r="54" spans="1:3" ht="40" customHeight="1">
-      <c r="A54" s="123"/>
-      <c r="B54" s="64"/>
+    <row r="54" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="170"/>
+      <c r="B54" s="63"/>
       <c r="C54" s="55"/>
     </row>
-    <row r="55" spans="1:3" ht="40" customHeight="1">
-      <c r="A55" s="119"/>
-      <c r="B55" s="63"/>
+    <row r="55" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="169"/>
+      <c r="B55" s="62"/>
       <c r="C55" s="55"/>
     </row>
-    <row r="56" spans="1:3" ht="40" customHeight="1">
-      <c r="A56" s="134"/>
-      <c r="B56" s="63"/>
+    <row r="56" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="185"/>
+      <c r="B56" s="62"/>
       <c r="C56" s="55"/>
     </row>
-    <row r="57" spans="1:3" ht="40" customHeight="1">
-      <c r="A57" s="144"/>
-      <c r="B57" s="63"/>
+    <row r="57" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="100"/>
+      <c r="B57" s="62"/>
       <c r="C57" s="55"/>
     </row>
-    <row r="58" spans="1:3" ht="40" customHeight="1">
-      <c r="A58" s="123"/>
-      <c r="B58" s="63"/>
+    <row r="58" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="170"/>
+      <c r="B58" s="62"/>
       <c r="C58" s="55"/>
     </row>
-    <row r="59" spans="1:3" ht="40" customHeight="1">
-      <c r="A59" s="89"/>
-      <c r="B59" s="63"/>
+    <row r="59" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="88"/>
+      <c r="B59" s="62"/>
       <c r="C59" s="55"/>
     </row>
-    <row r="60" spans="1:3" ht="40" customHeight="1">
-      <c r="A60" s="126"/>
+    <row r="60" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="183"/>
       <c r="B60" s="28"/>
       <c r="C60" s="55"/>
     </row>
-    <row r="61" spans="1:3" ht="40" customHeight="1">
-      <c r="A61" s="135"/>
+    <row r="61" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="171"/>
       <c r="B61" s="60"/>
       <c r="C61" s="55"/>
     </row>
-    <row r="62" spans="1:3" ht="40" customHeight="1">
-      <c r="A62" s="136"/>
+    <row r="62" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="186"/>
       <c r="B62" s="60"/>
       <c r="C62" s="55"/>
     </row>
-    <row r="63" spans="1:3" ht="40" customHeight="1">
-      <c r="A63" s="136"/>
+    <row r="63" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="186"/>
       <c r="B63" s="60"/>
       <c r="C63" s="55"/>
     </row>
-    <row r="64" spans="1:3" ht="40" customHeight="1">
-      <c r="A64" s="137"/>
+    <row r="64" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="187"/>
       <c r="B64" s="60"/>
       <c r="C64" s="55"/>
     </row>
-    <row r="65" spans="1:3" ht="40" customHeight="1">
-      <c r="A65" s="120"/>
+    <row r="65" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="174"/>
       <c r="B65" s="60"/>
       <c r="C65" s="59"/>
     </row>
-    <row r="66" spans="1:3" ht="40" customHeight="1">
-      <c r="A66" s="126"/>
+    <row r="66" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="183"/>
       <c r="B66" s="60"/>
       <c r="C66" s="55"/>
     </row>
-    <row r="67" spans="1:3" ht="40" customHeight="1">
-      <c r="A67" s="126"/>
+    <row r="67" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="183"/>
       <c r="B67" s="60"/>
       <c r="C67" s="55"/>
     </row>
-    <row r="68" spans="1:3" ht="40" customHeight="1">
-      <c r="A68" s="138"/>
+    <row r="68" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="177"/>
       <c r="B68" s="60"/>
       <c r="C68" s="55"/>
     </row>
-    <row r="69" spans="1:3" ht="40" customHeight="1">
-      <c r="A69" s="126"/>
+    <row r="69" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="183"/>
       <c r="B69" s="60"/>
       <c r="C69" s="55"/>
     </row>
-    <row r="70" spans="1:3" ht="40" customHeight="1">
-      <c r="A70" s="138"/>
+    <row r="70" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="177"/>
       <c r="B70" s="60"/>
       <c r="C70" s="55"/>
     </row>
-    <row r="71" spans="1:3" ht="40" customHeight="1">
-      <c r="A71" s="127"/>
+    <row r="71" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="188"/>
       <c r="B71" s="60"/>
       <c r="C71" s="55"/>
     </row>
-    <row r="72" spans="1:3" ht="40" customHeight="1">
-      <c r="A72" s="128"/>
+    <row r="72" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="189"/>
       <c r="C72" s="55"/>
     </row>
   </sheetData>
@@ -5757,14 +5744,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c298f69c-7e32-4d69-8a4f-44b776bc75e5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="27d18e64-52d1-4030-b5cf-9c691bb829da" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6005,21 +5990,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c298f69c-7e32-4d69-8a4f-44b776bc75e5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="27d18e64-52d1-4030-b5cf-9c691bb829da" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B37A3888-C326-48DF-AE4A-829BED1A658A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18B17227-D4F1-4BA2-A533-34BDC1F9C7F0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c298f69c-7e32-4d69-8a4f-44b776bc75e5"/>
-    <ds:schemaRef ds:uri="27d18e64-52d1-4030-b5cf-9c691bb829da"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6044,9 +6028,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18B17227-D4F1-4BA2-A533-34BDC1F9C7F0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B37A3888-C326-48DF-AE4A-829BED1A658A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c298f69c-7e32-4d69-8a4f-44b776bc75e5"/>
+    <ds:schemaRef ds:uri="27d18e64-52d1-4030-b5cf-9c691bb829da"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>